<commit_message>
Updated stats: Axes/Bardiches and blunt weapons.
</commit_message>
<xml_diff>
--- a/Items+Troops Spreadsheets/HYW Item Balance.xlsx
+++ b/Items+Troops Spreadsheets/HYW Item Balance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoanne\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoanne\Desktop\HYW Repo\Items+Troops Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8521E7AC-A1DE-4089-B44C-81FB6981C5D8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85557B73-AF25-4821-81EA-B444EC72173B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="2" activeTab="3" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
   </bookViews>
   <sheets>
     <sheet name="Maces" sheetId="1" r:id="rId1"/>
@@ -694,17 +694,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1030,7 +1050,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,31 +1060,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1075,15 +1095,25 @@
       <c r="B2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="3">
+      <c r="C2" s="9">
+        <v>4</v>
+      </c>
+      <c r="D2" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12">
+        <v>99</v>
+      </c>
+      <c r="G2" s="13">
         <v>63</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="H2" s="14">
+        <v>13</v>
+      </c>
+      <c r="I2" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1092,15 +1122,25 @@
       <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="3">
+      <c r="C3" s="9">
+        <v>77</v>
+      </c>
+      <c r="D3" s="10">
+        <v>2</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12">
+        <v>99</v>
+      </c>
+      <c r="G3" s="13">
         <v>73</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="H3" s="14">
+        <v>20</v>
+      </c>
+      <c r="I3" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1109,15 +1149,25 @@
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="3">
+      <c r="C4" s="9">
+        <v>293</v>
+      </c>
+      <c r="D4" s="10">
+        <v>2</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12">
+        <v>95</v>
+      </c>
+      <c r="G4" s="13">
         <v>70</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="H4" s="14">
+        <v>30</v>
+      </c>
+      <c r="I4" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1126,15 +1176,25 @@
       <c r="B5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="3">
+      <c r="C5" s="9">
+        <v>317</v>
+      </c>
+      <c r="D5" s="10">
+        <v>2</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12">
+        <v>95</v>
+      </c>
+      <c r="G5" s="13">
         <v>70</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="H5" s="14">
+        <v>31</v>
+      </c>
+      <c r="I5" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1143,15 +1203,25 @@
       <c r="B6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="3">
+      <c r="C6" s="9">
+        <v>372</v>
+      </c>
+      <c r="D6" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12">
+        <v>95</v>
+      </c>
+      <c r="G6" s="13">
         <v>76</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="H6" s="14">
+        <v>33</v>
+      </c>
+      <c r="I6" s="14">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -1160,15 +1230,25 @@
       <c r="B7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="3">
+      <c r="C7" s="9">
+        <v>334</v>
+      </c>
+      <c r="D7" s="10">
+        <v>2</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12">
+        <v>95</v>
+      </c>
+      <c r="G7" s="13">
         <v>63</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="H7" s="14">
+        <v>32</v>
+      </c>
+      <c r="I7" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1177,15 +1257,27 @@
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="3">
+      <c r="C8" s="9">
+        <v>422</v>
+      </c>
+      <c r="D8" s="10">
+        <v>9</v>
+      </c>
+      <c r="E8" s="11">
+        <v>14</v>
+      </c>
+      <c r="F8" s="12">
+        <v>79</v>
+      </c>
+      <c r="G8" s="13">
         <v>75</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="H8" s="14">
+        <v>45</v>
+      </c>
+      <c r="I8" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -1194,15 +1286,25 @@
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="3">
+      <c r="C9" s="9">
+        <v>336</v>
+      </c>
+      <c r="D9" s="10">
+        <v>4</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12">
+        <v>96</v>
+      </c>
+      <c r="G9" s="13">
         <v>69</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="H9" s="14">
+        <v>28</v>
+      </c>
+      <c r="I9" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -1211,15 +1313,25 @@
       <c r="B10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="3">
+      <c r="C10" s="9">
+        <v>262</v>
+      </c>
+      <c r="D10" s="10">
+        <v>3.25</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="12">
+        <v>97</v>
+      </c>
+      <c r="G10" s="13">
         <v>72</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="H10" s="14">
+        <v>26</v>
+      </c>
+      <c r="I10" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -1228,15 +1340,25 @@
       <c r="B11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="3">
+      <c r="C11" s="9">
+        <v>83</v>
+      </c>
+      <c r="D11" s="10">
+        <v>3.25</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="12">
+        <v>96</v>
+      </c>
+      <c r="G11" s="13">
         <v>75</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="H11" s="14">
+        <v>21</v>
+      </c>
+      <c r="I11" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -1245,15 +1367,25 @@
       <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="3">
+      <c r="C12" s="9">
+        <v>98</v>
+      </c>
+      <c r="D12" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="12">
+        <v>98</v>
+      </c>
+      <c r="G12" s="13">
         <v>70</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="H12" s="14">
+        <v>21</v>
+      </c>
+      <c r="I12" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -1262,15 +1394,25 @@
       <c r="B13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="3">
+      <c r="C13" s="9">
+        <v>152</v>
+      </c>
+      <c r="D13" s="10">
+        <v>2.75</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12">
+        <v>98</v>
+      </c>
+      <c r="G13" s="13">
         <v>71</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="H13" s="14">
+        <v>23</v>
+      </c>
+      <c r="I13" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -1279,15 +1421,25 @@
       <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="3">
+      <c r="C14" s="9">
+        <v>212</v>
+      </c>
+      <c r="D14" s="10">
+        <v>3</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="12">
+        <v>97</v>
+      </c>
+      <c r="G14" s="13">
         <v>71</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="H14" s="14">
+        <v>24</v>
+      </c>
+      <c r="I14" s="14">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1296,10 +1448,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64CAC7F2-FAD3-4FE8-9D42-216993956934}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,31 +1461,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1344,15 +1496,25 @@
       <c r="B2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="3">
+      <c r="C2" s="15">
+        <v>71</v>
+      </c>
+      <c r="D2" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12">
+        <v>98</v>
+      </c>
+      <c r="G2" s="13">
         <v>46</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="H2" s="14">
+        <v>21</v>
+      </c>
+      <c r="I2" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1361,15 +1523,25 @@
       <c r="B3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="3">
+      <c r="C3" s="15">
+        <v>221</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1.75</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12">
+        <v>97</v>
+      </c>
+      <c r="G3" s="13">
         <v>70</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="H3" s="14">
+        <v>34</v>
+      </c>
+      <c r="I3" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1378,15 +1550,25 @@
       <c r="B4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="3">
+      <c r="C4" s="15">
+        <v>87</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12">
+        <v>96</v>
+      </c>
+      <c r="G4" s="13">
         <v>71</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="H4" s="14">
+        <v>32</v>
+      </c>
+      <c r="I4" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1395,15 +1577,25 @@
       <c r="B5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="3">
+      <c r="C5" s="15">
+        <v>142</v>
+      </c>
+      <c r="D5" s="10">
+        <v>2</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12">
+        <v>95</v>
+      </c>
+      <c r="G5" s="13">
         <v>71</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="H5" s="14">
+        <v>33</v>
+      </c>
+      <c r="I5" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1412,338 +1604,571 @@
       <c r="B6" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="3">
+      <c r="C6" s="15">
+        <v>190</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1.75</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12">
+        <v>96</v>
+      </c>
+      <c r="G6" s="13">
         <v>73</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="H6" s="14">
+        <v>34</v>
+      </c>
+      <c r="I6" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="3">
-        <v>77</v>
-      </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="3">
-        <v>73</v>
-      </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="C8" s="15">
+        <v>202</v>
+      </c>
+      <c r="D8" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12">
+        <v>98</v>
+      </c>
+      <c r="G8" s="13">
+        <v>77</v>
+      </c>
+      <c r="H8" s="14">
+        <v>31</v>
+      </c>
+      <c r="I8" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="3">
-        <v>79</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="C9" s="15">
+        <v>176</v>
+      </c>
+      <c r="D9" s="10">
+        <v>1.75</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12">
+        <v>97</v>
+      </c>
+      <c r="G9" s="13">
+        <v>73</v>
+      </c>
+      <c r="H9" s="14">
+        <v>30</v>
+      </c>
+      <c r="I9" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="3">
-        <v>94</v>
-      </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="C10" s="15">
+        <v>234</v>
+      </c>
+      <c r="D10" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="12">
+        <v>97</v>
+      </c>
+      <c r="G10" s="13">
+        <v>79</v>
+      </c>
+      <c r="H10" s="14">
+        <v>32</v>
+      </c>
+      <c r="I10" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="3">
-        <v>79</v>
-      </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="C11" s="15">
+        <v>354</v>
+      </c>
+      <c r="D11" s="10">
+        <v>3</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="12">
+        <v>94</v>
+      </c>
+      <c r="G11" s="13">
+        <v>94</v>
+      </c>
+      <c r="H11" s="14">
+        <v>35</v>
+      </c>
+      <c r="I11" s="14">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="3">
-        <v>97</v>
-      </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="C12" s="15">
+        <v>246</v>
+      </c>
+      <c r="D12" s="10">
+        <v>2</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="12">
+        <v>96</v>
+      </c>
+      <c r="G12" s="13">
+        <v>79</v>
+      </c>
+      <c r="H12" s="14">
+        <v>34</v>
+      </c>
+      <c r="I12" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="3">
-        <v>99</v>
-      </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="C13" s="15">
+        <v>371</v>
+      </c>
+      <c r="D13" s="10">
+        <v>3</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12">
+        <v>94</v>
+      </c>
+      <c r="G13" s="13">
+        <v>97</v>
+      </c>
+      <c r="H13" s="14">
+        <v>36</v>
+      </c>
+      <c r="I13" s="14">
+        <v>18</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="3">
-        <v>98</v>
-      </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="3">
+      <c r="C15" s="15">
+        <v>236</v>
+      </c>
+      <c r="D15" s="10">
+        <v>3.5</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12">
+        <v>95</v>
+      </c>
+      <c r="G15" s="13">
         <v>99</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="H15" s="14">
+        <v>41</v>
+      </c>
+      <c r="I15" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="3">
-        <v>156</v>
-      </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="C16" s="15">
+        <v>287</v>
+      </c>
+      <c r="D16" s="10">
+        <v>4</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="12">
+        <v>94</v>
+      </c>
+      <c r="G16" s="13">
+        <v>98</v>
+      </c>
+      <c r="H16" s="14">
+        <v>43</v>
+      </c>
+      <c r="I16" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="3">
-        <v>140</v>
-      </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="C17" s="15">
+        <v>321</v>
+      </c>
+      <c r="D17" s="10">
+        <v>4</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="12">
+        <v>94</v>
+      </c>
+      <c r="G17" s="13">
+        <v>99</v>
+      </c>
+      <c r="H17" s="14">
+        <v>44</v>
+      </c>
+      <c r="I17" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="3">
-        <v>155</v>
-      </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="C18" s="15">
+        <v>304</v>
+      </c>
+      <c r="D18" s="10">
+        <v>4</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="12">
+        <v>90</v>
+      </c>
+      <c r="G18" s="13">
+        <v>156</v>
+      </c>
+      <c r="H18" s="14">
+        <v>39</v>
+      </c>
+      <c r="I18" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="3">
-        <v>107</v>
-      </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="3">
-        <v>103</v>
-      </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="C20" s="15">
+        <v>539</v>
+      </c>
+      <c r="D20" s="10">
+        <v>5.75</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="12">
+        <v>86</v>
+      </c>
+      <c r="G20" s="13">
+        <v>140</v>
+      </c>
+      <c r="H20" s="14">
+        <v>51</v>
+      </c>
+      <c r="I20" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="3">
-        <v>106</v>
-      </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="C21" s="15">
+        <v>628</v>
+      </c>
+      <c r="D21" s="10">
+        <v>6</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="12">
+        <v>85</v>
+      </c>
+      <c r="G21" s="13">
+        <v>155</v>
+      </c>
+      <c r="H21" s="14">
+        <v>52</v>
+      </c>
+      <c r="I21" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="3">
-        <v>110</v>
-      </c>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
+      <c r="C22" s="15">
+        <v>334</v>
+      </c>
+      <c r="D22" s="10">
+        <v>5</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="12">
+        <v>89</v>
+      </c>
+      <c r="G22" s="13">
+        <v>107</v>
+      </c>
+      <c r="H22" s="14">
+        <v>45</v>
+      </c>
+      <c r="I22" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="3">
-        <v>106</v>
-      </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="C23" s="15">
+        <v>306</v>
+      </c>
+      <c r="D23" s="10">
+        <v>5</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="12">
+        <v>91</v>
+      </c>
+      <c r="G23" s="13">
+        <v>103</v>
+      </c>
+      <c r="H23" s="14">
+        <v>44</v>
+      </c>
+      <c r="I23" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="3">
-        <v>105</v>
-      </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
+      <c r="C24" s="15">
+        <v>368</v>
+      </c>
+      <c r="D24" s="10">
+        <v>5.25</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12">
+        <v>90</v>
+      </c>
+      <c r="G24" s="13">
+        <v>106</v>
+      </c>
+      <c r="H24" s="14">
+        <v>46</v>
+      </c>
+      <c r="I24" s="14">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="3">
+      <c r="C25" s="15">
+        <v>399</v>
+      </c>
+      <c r="D25" s="10">
+        <v>5.25</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="12">
+        <v>89</v>
+      </c>
+      <c r="G25" s="13">
+        <v>110</v>
+      </c>
+      <c r="H25" s="14">
+        <v>47</v>
+      </c>
+      <c r="I25" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="15">
+        <v>291</v>
+      </c>
+      <c r="D26" s="10">
+        <v>5</v>
+      </c>
+      <c r="E26" s="11"/>
+      <c r="F26" s="12">
+        <v>91</v>
+      </c>
+      <c r="G26" s="13">
+        <v>106</v>
+      </c>
+      <c r="H26" s="14">
+        <v>43</v>
+      </c>
+      <c r="I26" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="15">
+        <v>498</v>
+      </c>
+      <c r="D27" s="10">
+        <v>5.5</v>
+      </c>
+      <c r="E27" s="11"/>
+      <c r="F27" s="12">
+        <v>88</v>
+      </c>
+      <c r="G27" s="13">
+        <v>105</v>
+      </c>
+      <c r="H27" s="14">
+        <v>49</v>
+      </c>
+      <c r="I27" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="15">
+        <v>464</v>
+      </c>
+      <c r="D28" s="10">
+        <v>5.5</v>
+      </c>
+      <c r="E28" s="11"/>
+      <c r="F28" s="12">
+        <v>89</v>
+      </c>
+      <c r="G28" s="13">
         <v>101</v>
       </c>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
+      <c r="H28" s="14">
+        <v>48</v>
+      </c>
+      <c r="I28" s="14">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1766,31 +2191,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1801,10 +2226,10 @@
       <c r="B2" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="5"/>
       <c r="G2" s="3">
         <v>47</v>
       </c>
@@ -1818,10 +2243,10 @@
       <c r="B3" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="3">
         <v>41</v>
       </c>
@@ -1835,10 +2260,10 @@
       <c r="B4" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="3">
         <v>47</v>
       </c>
@@ -1848,10 +2273,10 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="3"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1863,10 +2288,10 @@
       <c r="B6" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="5"/>
       <c r="G6" s="3">
         <v>70</v>
       </c>
@@ -1880,10 +2305,10 @@
       <c r="B7" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="5"/>
       <c r="G7" s="3">
         <v>95</v>
       </c>
@@ -1897,10 +2322,10 @@
       <c r="B8" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="3">
         <v>101</v>
       </c>
@@ -1914,10 +2339,10 @@
       <c r="B9" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="3">
         <v>95</v>
       </c>
@@ -1931,10 +2356,10 @@
       <c r="B10" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="3">
         <v>101</v>
       </c>
@@ -1948,10 +2373,10 @@
       <c r="B11" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="5"/>
       <c r="G11" s="3">
         <v>81</v>
       </c>
@@ -1965,10 +2390,10 @@
       <c r="B12" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="3">
         <v>95</v>
       </c>
@@ -1982,10 +2407,10 @@
       <c r="B13" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="3">
         <v>101</v>
       </c>
@@ -1999,10 +2424,10 @@
       <c r="B14" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="3">
         <v>98</v>
       </c>
@@ -2016,10 +2441,10 @@
       <c r="B15" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="5"/>
       <c r="G15" s="3">
         <v>74</v>
       </c>
@@ -2033,10 +2458,10 @@
       <c r="B16" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="5"/>
       <c r="G16" s="3">
         <v>81</v>
       </c>
@@ -2046,10 +2471,10 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="5"/>
       <c r="G17" s="3"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -2061,10 +2486,10 @@
       <c r="B18" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="5"/>
       <c r="G18" s="3">
         <v>85</v>
       </c>
@@ -2078,10 +2503,10 @@
       <c r="B19" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="5"/>
       <c r="G19" s="3">
         <v>93</v>
       </c>
@@ -2095,10 +2520,10 @@
       <c r="B20" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="5"/>
       <c r="G20" s="3">
         <v>103</v>
       </c>
@@ -2112,10 +2537,10 @@
       <c r="B21" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="5"/>
       <c r="G21" s="3">
         <v>97</v>
       </c>
@@ -2129,10 +2554,10 @@
       <c r="B22" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="5"/>
       <c r="G22" s="3">
         <v>99</v>
       </c>
@@ -2146,10 +2571,10 @@
       <c r="B23" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="3">
         <v>100</v>
       </c>
@@ -2163,10 +2588,10 @@
       <c r="B24" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="5"/>
       <c r="G24" s="3">
         <v>99</v>
       </c>
@@ -2180,10 +2605,10 @@
       <c r="B25" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="5"/>
       <c r="G25" s="3">
         <v>107</v>
       </c>
@@ -2197,10 +2622,10 @@
       <c r="B26" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="5"/>
       <c r="G26" s="3">
         <v>93</v>
       </c>
@@ -2214,10 +2639,10 @@
       <c r="B27" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="5"/>
       <c r="G27" s="3">
         <v>93</v>
       </c>
@@ -2231,10 +2656,10 @@
       <c r="B28" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="5"/>
       <c r="G28" s="3">
         <v>83</v>
       </c>
@@ -2248,10 +2673,10 @@
       <c r="B29" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="5"/>
       <c r="G29" s="3">
         <v>92</v>
       </c>
@@ -2265,10 +2690,10 @@
       <c r="B30" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="5"/>
       <c r="G30" s="3">
         <v>96</v>
       </c>
@@ -2282,10 +2707,10 @@
       <c r="B31" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="5"/>
       <c r="G31" s="3">
         <v>102</v>
       </c>
@@ -2299,10 +2724,10 @@
       <c r="B32" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="5"/>
       <c r="G32" s="3">
         <v>83</v>
       </c>
@@ -2316,10 +2741,10 @@
       <c r="B33" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="5"/>
       <c r="G33" s="3">
         <v>97</v>
       </c>
@@ -2333,10 +2758,10 @@
       <c r="B34" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="5"/>
       <c r="G34" s="3">
         <v>102</v>
       </c>
@@ -2352,7 +2777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03FAF929-B978-461F-BC5C-F0B53573D36C}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -2363,31 +2788,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2398,10 +2823,10 @@
       <c r="B2" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="5"/>
       <c r="G2" s="3">
         <v>99</v>
       </c>
@@ -2415,10 +2840,10 @@
       <c r="B3" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="3">
         <v>104</v>
       </c>
@@ -2432,10 +2857,10 @@
       <c r="B4" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="3">
         <v>104</v>
       </c>
@@ -2449,10 +2874,10 @@
       <c r="B5" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="3">
         <v>101</v>
       </c>
@@ -2466,10 +2891,10 @@
       <c r="B6" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="5"/>
       <c r="G6" s="3">
         <v>106</v>
       </c>
@@ -2483,10 +2908,10 @@
       <c r="B7" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="5"/>
       <c r="G7" s="3">
         <v>107</v>
       </c>
@@ -2496,10 +2921,10 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="3"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -2511,10 +2936,10 @@
       <c r="B9" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="3">
         <v>99</v>
       </c>
@@ -2528,10 +2953,10 @@
       <c r="B10" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="3">
         <v>111</v>
       </c>
@@ -2545,10 +2970,10 @@
       <c r="B11" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="5"/>
       <c r="G11" s="3">
         <v>110</v>
       </c>
@@ -2562,10 +2987,10 @@
       <c r="B12" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="3">
         <v>100</v>
       </c>
@@ -2579,10 +3004,10 @@
       <c r="B13" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="3">
         <v>107</v>
       </c>
@@ -2596,10 +3021,10 @@
       <c r="B14" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="3">
         <v>106</v>
       </c>
@@ -2613,10 +3038,10 @@
       <c r="B15" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="5"/>
       <c r="G15" s="3">
         <v>109</v>
       </c>
@@ -2630,10 +3055,10 @@
       <c r="B16" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="5"/>
       <c r="G16" s="3">
         <v>101</v>
       </c>
@@ -2647,10 +3072,10 @@
       <c r="B17" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="5"/>
       <c r="G17" s="3">
         <v>109</v>
       </c>
@@ -2664,10 +3089,10 @@
       <c r="B18" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="5"/>
       <c r="G18" s="3">
         <v>109</v>
       </c>
@@ -2677,10 +3102,10 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="5"/>
       <c r="G19" s="3"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -2692,10 +3117,10 @@
       <c r="B20" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="5"/>
       <c r="G20" s="3">
         <v>93</v>
       </c>
@@ -2709,10 +3134,10 @@
       <c r="B21" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="5"/>
       <c r="G21" s="3">
         <v>115</v>
       </c>
@@ -2726,10 +3151,10 @@
       <c r="B22" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="5"/>
       <c r="G22" s="3">
         <v>114</v>
       </c>
@@ -2743,10 +3168,10 @@
       <c r="B23" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="3">
         <v>99</v>
       </c>
@@ -2760,10 +3185,10 @@
       <c r="B24" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="5"/>
       <c r="G24" s="3">
         <v>115</v>
       </c>
@@ -2789,31 +3214,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2822,10 +3247,10 @@
         <v>119</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="5"/>
       <c r="G2" s="3"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -2835,10 +3260,10 @@
         <v>120</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="3"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -2848,10 +3273,10 @@
         <v>121</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="3"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -2861,10 +3286,10 @@
         <v>122</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="3"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -2874,10 +3299,10 @@
         <v>123</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="5"/>
       <c r="G6" s="3"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -2887,10 +3312,10 @@
         <v>124</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="5"/>
       <c r="G7" s="3"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -2900,10 +3325,10 @@
         <v>125</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="3"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -2913,10 +3338,10 @@
         <v>126</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="3"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -2926,10 +3351,10 @@
         <v>127</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="3"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -2939,10 +3364,10 @@
         <v>128</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="3"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -2952,10 +3377,10 @@
         <v>129</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="3"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -2965,10 +3390,10 @@
         <v>130</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="3"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -2978,10 +3403,10 @@
         <v>131</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="5"/>
       <c r="G15" s="3"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -2991,10 +3416,10 @@
         <v>132</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="5"/>
       <c r="G16" s="3"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -3004,10 +3429,10 @@
         <v>133</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="5"/>
       <c r="G17" s="3"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -3017,10 +3442,10 @@
         <v>134</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="5"/>
       <c r="G18" s="3"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -3030,10 +3455,10 @@
         <v>135</v>
       </c>
       <c r="B19" s="2"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="5"/>
       <c r="G19" s="3"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -3043,10 +3468,10 @@
         <v>136</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="5"/>
       <c r="G20" s="3"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -3056,10 +3481,10 @@
         <v>137</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="5"/>
       <c r="G21" s="3"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -3069,10 +3494,10 @@
         <v>138</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="5"/>
       <c r="G22" s="3"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -3082,10 +3507,10 @@
         <v>139</v>
       </c>
       <c r="B23" s="2"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="3"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -3095,10 +3520,10 @@
         <v>140</v>
       </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="5"/>
       <c r="G24" s="3"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -3108,10 +3533,10 @@
         <v>141</v>
       </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="5"/>
       <c r="G25" s="3"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>

</xml_diff>

<commit_message>
Updated ranged weapons stats, minor tweaks to some troops.
</commit_message>
<xml_diff>
--- a/Items+Troops Spreadsheets/HYW Item Balance.xlsx
+++ b/Items+Troops Spreadsheets/HYW Item Balance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoanne\Desktop\HYW Repo\Items+Troops Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85557B73-AF25-4821-81EA-B444EC72173B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A41F0C-0128-48E3-8A20-95260CA0CB02}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="4" activeTab="5" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
   </bookViews>
   <sheets>
     <sheet name="Maces" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Swords &amp; Daggers" sheetId="3" r:id="rId3"/>
     <sheet name="Bastard &amp; Twohanded Swords" sheetId="4" r:id="rId4"/>
     <sheet name="Pikes &amp; Halberds &amp; Voulges" sheetId="5" r:id="rId5"/>
+    <sheet name="Bows" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="214">
   <si>
     <t>ID</t>
   </si>
@@ -590,6 +591,87 @@
   </si>
   <si>
     <t>Talhoffer Greatsword</t>
+  </si>
+  <si>
+    <t>Draw Speed</t>
+  </si>
+  <si>
+    <t>Projectile Speed</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>w_hunting_bow_ash</t>
+  </si>
+  <si>
+    <t>w_hunting_bow_elm</t>
+  </si>
+  <si>
+    <t>w_hunting_bow_oak</t>
+  </si>
+  <si>
+    <t>w_hunting_bow_yew</t>
+  </si>
+  <si>
+    <t>w_short_bow_ash</t>
+  </si>
+  <si>
+    <t>w_short_bow_elm</t>
+  </si>
+  <si>
+    <t>w_short_bow_oak</t>
+  </si>
+  <si>
+    <t>w_short_bow_yew</t>
+  </si>
+  <si>
+    <t>w_long_bow_ash</t>
+  </si>
+  <si>
+    <t>w_long_bow_elm</t>
+  </si>
+  <si>
+    <t>w_long_bow_oak</t>
+  </si>
+  <si>
+    <t>w_long_bow_yew</t>
+  </si>
+  <si>
+    <t>w_war_bow_ash</t>
+  </si>
+  <si>
+    <t>w_war_bow_elm</t>
+  </si>
+  <si>
+    <t>w_war_bow_oak</t>
+  </si>
+  <si>
+    <t>w_war_bow_yew</t>
+  </si>
+  <si>
+    <t>hunting_crossbow</t>
+  </si>
+  <si>
+    <t>light_crossbow</t>
+  </si>
+  <si>
+    <t>crossbow</t>
+  </si>
+  <si>
+    <t>heavy_crossbow</t>
+  </si>
+  <si>
+    <t>sniper_crossbow</t>
+  </si>
+  <si>
+    <t>w_handgonne_1</t>
+  </si>
+  <si>
+    <t>w_handgonne_2</t>
   </si>
 </sst>
 </file>
@@ -1450,8 +1532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64CAC7F2-FAD3-4FE8-9D42-216993956934}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3205,7 +3287,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3544,4 +3626,674 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96551E4B-D0DF-400F-B6DB-43F70FA502C4}">
+  <dimension ref="A1:I29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="6">
+        <v>42</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>95</v>
+      </c>
+      <c r="G2" s="3">
+        <v>40</v>
+      </c>
+      <c r="H2" s="1">
+        <v>90</v>
+      </c>
+      <c r="I2" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="6">
+        <v>50</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>94</v>
+      </c>
+      <c r="G3" s="3">
+        <v>42</v>
+      </c>
+      <c r="H3" s="1">
+        <v>90</v>
+      </c>
+      <c r="I3" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="6">
+        <v>58</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>93</v>
+      </c>
+      <c r="G4" s="3">
+        <v>44</v>
+      </c>
+      <c r="H4" s="1">
+        <v>91</v>
+      </c>
+      <c r="I4" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="6">
+        <v>66</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>92</v>
+      </c>
+      <c r="G5" s="3">
+        <v>45</v>
+      </c>
+      <c r="H5" s="1">
+        <v>92</v>
+      </c>
+      <c r="I5" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="6">
+        <v>90</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5">
+        <v>90</v>
+      </c>
+      <c r="G7" s="3">
+        <v>45</v>
+      </c>
+      <c r="H7" s="1">
+        <v>92</v>
+      </c>
+      <c r="I7" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="6">
+        <v>102</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5">
+        <v>89</v>
+      </c>
+      <c r="G8" s="3">
+        <v>48</v>
+      </c>
+      <c r="H8" s="1">
+        <v>92</v>
+      </c>
+      <c r="I8" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="6">
+        <v>124</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E9" s="7">
+        <v>2</v>
+      </c>
+      <c r="F9" s="5">
+        <v>88</v>
+      </c>
+      <c r="G9" s="3">
+        <v>51</v>
+      </c>
+      <c r="H9" s="1">
+        <v>93</v>
+      </c>
+      <c r="I9" s="4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="6">
+        <v>136</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="7">
+        <v>2</v>
+      </c>
+      <c r="F10" s="5">
+        <v>87</v>
+      </c>
+      <c r="G10" s="3">
+        <v>54</v>
+      </c>
+      <c r="H10" s="1">
+        <v>94</v>
+      </c>
+      <c r="I10" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="6">
+        <v>140</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="E12" s="7">
+        <v>3</v>
+      </c>
+      <c r="F12" s="5">
+        <v>85</v>
+      </c>
+      <c r="G12" s="3">
+        <v>71</v>
+      </c>
+      <c r="H12" s="1">
+        <v>95</v>
+      </c>
+      <c r="I12" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="6">
+        <v>154</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="E13" s="7">
+        <v>3</v>
+      </c>
+      <c r="F13" s="5">
+        <v>84</v>
+      </c>
+      <c r="G13" s="3">
+        <v>76</v>
+      </c>
+      <c r="H13" s="1">
+        <v>95</v>
+      </c>
+      <c r="I13" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="6">
+        <v>168</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="E14" s="7">
+        <v>3</v>
+      </c>
+      <c r="F14" s="5">
+        <v>83</v>
+      </c>
+      <c r="G14" s="3">
+        <v>82</v>
+      </c>
+      <c r="H14" s="1">
+        <v>96</v>
+      </c>
+      <c r="I14" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="6">
+        <v>184</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E15" s="7">
+        <v>3</v>
+      </c>
+      <c r="F15" s="5">
+        <v>82</v>
+      </c>
+      <c r="G15" s="3">
+        <v>89</v>
+      </c>
+      <c r="H15" s="1">
+        <v>97</v>
+      </c>
+      <c r="I15" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="6">
+        <v>220</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E17" s="7">
+        <v>4</v>
+      </c>
+      <c r="F17" s="5">
+        <v>80</v>
+      </c>
+      <c r="G17" s="3">
+        <v>107</v>
+      </c>
+      <c r="H17" s="1">
+        <v>98</v>
+      </c>
+      <c r="I17" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="6">
+        <v>235</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E18" s="7">
+        <v>4</v>
+      </c>
+      <c r="F18" s="5">
+        <v>79</v>
+      </c>
+      <c r="G18" s="3">
+        <v>115</v>
+      </c>
+      <c r="H18" s="1">
+        <v>98</v>
+      </c>
+      <c r="I18" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="6">
+        <v>250</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E19" s="7">
+        <v>5</v>
+      </c>
+      <c r="F19" s="5">
+        <v>78</v>
+      </c>
+      <c r="G19" s="3">
+        <v>128</v>
+      </c>
+      <c r="H19" s="1">
+        <v>99</v>
+      </c>
+      <c r="I19" s="4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="6">
+        <v>265</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="E20" s="7">
+        <v>5</v>
+      </c>
+      <c r="F20" s="5">
+        <v>77</v>
+      </c>
+      <c r="G20" s="3">
+        <v>134</v>
+      </c>
+      <c r="H20" s="1">
+        <v>99</v>
+      </c>
+      <c r="I20" s="4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="6">
+        <v>88</v>
+      </c>
+      <c r="D22" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5">
+        <v>80</v>
+      </c>
+      <c r="G22" s="3">
+        <v>81</v>
+      </c>
+      <c r="H22" s="1">
+        <v>98</v>
+      </c>
+      <c r="I22" s="4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="6">
+        <v>132</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="E23" s="7">
+        <v>8</v>
+      </c>
+      <c r="F23" s="5">
+        <v>76</v>
+      </c>
+      <c r="G23" s="3">
+        <v>92</v>
+      </c>
+      <c r="H23" s="1">
+        <v>98</v>
+      </c>
+      <c r="I23" s="4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="6">
+        <v>218</v>
+      </c>
+      <c r="D24" s="4">
+        <v>3</v>
+      </c>
+      <c r="E24" s="7">
+        <v>9</v>
+      </c>
+      <c r="F24" s="5">
+        <v>72</v>
+      </c>
+      <c r="G24" s="3">
+        <v>124</v>
+      </c>
+      <c r="H24" s="1">
+        <v>99</v>
+      </c>
+      <c r="I24" s="4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="6">
+        <v>349</v>
+      </c>
+      <c r="D25" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="E25" s="7">
+        <v>10</v>
+      </c>
+      <c r="F25" s="5">
+        <v>68</v>
+      </c>
+      <c r="G25" s="3">
+        <v>139</v>
+      </c>
+      <c r="H25" s="1">
+        <v>99</v>
+      </c>
+      <c r="I25" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="6">
+        <v>683</v>
+      </c>
+      <c r="D26" s="4">
+        <v>3.75</v>
+      </c>
+      <c r="E26" s="7">
+        <v>11</v>
+      </c>
+      <c r="F26" s="5">
+        <v>62</v>
+      </c>
+      <c r="G26" s="3">
+        <v>142</v>
+      </c>
+      <c r="H26" s="1">
+        <v>98</v>
+      </c>
+      <c r="I26" s="4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="6">
+        <v>1850</v>
+      </c>
+      <c r="D28" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="E28" s="7">
+        <v>0</v>
+      </c>
+      <c r="F28" s="5">
+        <v>58</v>
+      </c>
+      <c r="G28" s="3">
+        <v>160</v>
+      </c>
+      <c r="H28" s="1">
+        <v>95</v>
+      </c>
+      <c r="I28" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="6">
+        <v>2250</v>
+      </c>
+      <c r="D29" s="4">
+        <v>3.8</v>
+      </c>
+      <c r="E29" s="7">
+        <v>0</v>
+      </c>
+      <c r="F29" s="5">
+        <v>60</v>
+      </c>
+      <c r="G29" s="3">
+        <v>180</v>
+      </c>
+      <c r="H29" s="1">
+        <v>98</v>
+      </c>
+      <c r="I29" s="4">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Further rebalancing of items, added variants to most armors from HYW_plate_armors.brf. "Stable" update before re-implementing banners.
</commit_message>
<xml_diff>
--- a/Items+Troops Spreadsheets/HYW Item Balance.xlsx
+++ b/Items+Troops Spreadsheets/HYW Item Balance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoanne\Desktop\HYW Repo\Items+Troops Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A41F0C-0128-48E3-8A20-95260CA0CB02}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FCD007-7BD0-48D5-91FD-D1DAE592355A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="4" activeTab="5" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="1" activeTab="2" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
   </bookViews>
   <sheets>
     <sheet name="Maces" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,22 @@
     <sheet name="Pikes &amp; Halberds &amp; Voulges" sheetId="5" r:id="rId5"/>
     <sheet name="Bows" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="215">
   <si>
     <t>ID</t>
   </si>
@@ -672,6 +677,9 @@
   </si>
   <si>
     <t>w_handgonne_2</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -749,7 +757,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -772,11 +780,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -807,6 +826,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2261,9 +2281,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76258844-B7FB-4720-B431-7E6F0F318E31}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G35" sqref="G35"/>
+      <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2308,15 +2328,27 @@
       <c r="B2" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="5"/>
+      <c r="C2" s="6">
+        <v>73</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>103</v>
+      </c>
       <c r="G2" s="3">
         <v>47</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="H2" s="1">
+        <v>22</v>
+      </c>
+      <c r="I2" s="1">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2325,15 +2357,27 @@
       <c r="B3" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="5"/>
+      <c r="C3" s="6">
+        <v>122</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>105</v>
+      </c>
       <c r="G3" s="3">
         <v>41</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="H3" s="1">
+        <v>28</v>
+      </c>
+      <c r="I3" s="1">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -2342,15 +2386,27 @@
       <c r="B4" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="5"/>
+      <c r="C4" s="6">
+        <v>136</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>103</v>
+      </c>
       <c r="G4" s="3">
         <v>47</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="H4" s="1">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
@@ -2857,10 +2913,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03FAF929-B978-461F-BC5C-F0B53573D36C}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2869,7 +2925,7 @@
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2897,110 +2953,183 @@
       <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="16"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="5"/>
+      <c r="C2" s="6">
+        <v>294</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2</v>
+      </c>
+      <c r="E2" s="7">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5">
+        <v>98</v>
+      </c>
       <c r="G2" s="3">
         <v>99</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H2" s="1">
+        <v>35</v>
+      </c>
+      <c r="I2" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="5"/>
+      <c r="C3" s="6">
+        <v>526</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="E3" s="7">
+        <v>9</v>
+      </c>
+      <c r="F3" s="5">
+        <v>97</v>
+      </c>
       <c r="G3" s="3">
         <v>104</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H3" s="1">
+        <v>37</v>
+      </c>
+      <c r="I3" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="5"/>
+      <c r="C4" s="6">
+        <v>548</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="E4" s="7">
+        <v>9</v>
+      </c>
+      <c r="F4" s="5">
+        <v>97</v>
+      </c>
       <c r="G4" s="3">
         <v>104</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4" s="1">
+        <v>38</v>
+      </c>
+      <c r="I4" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="5"/>
+      <c r="C5" s="6">
+        <v>676</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
+      <c r="E5" s="7">
+        <v>9</v>
+      </c>
+      <c r="F5" s="5">
+        <v>99</v>
+      </c>
       <c r="G5" s="3">
         <v>101</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H5" s="1">
+        <v>37</v>
+      </c>
+      <c r="I5" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="5"/>
+      <c r="C6" s="6">
+        <v>724</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="E6" s="7">
+        <v>9</v>
+      </c>
+      <c r="F6" s="5">
+        <v>97</v>
+      </c>
       <c r="G6" s="3">
         <v>106</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6" s="1">
+        <v>38</v>
+      </c>
+      <c r="I6" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="5"/>
+      <c r="C7" s="6">
+        <v>638</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="E7" s="7">
+        <v>9</v>
+      </c>
+      <c r="F7" s="5">
+        <v>97</v>
+      </c>
       <c r="G7" s="3">
         <v>107</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H7" s="1">
+        <v>36</v>
+      </c>
+      <c r="I7" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="6"/>
@@ -3011,141 +3140,240 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="5"/>
+      <c r="C9" s="6">
+        <v>698</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="E9" s="7">
+        <v>9</v>
+      </c>
+      <c r="F9" s="5">
+        <v>98</v>
+      </c>
       <c r="G9" s="3">
         <v>99</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H9" s="1">
+        <v>38</v>
+      </c>
+      <c r="I9" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="5"/>
+      <c r="C10" s="6">
+        <v>892</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2.75</v>
+      </c>
+      <c r="E10" s="7">
+        <v>9</v>
+      </c>
+      <c r="F10" s="5">
+        <v>96</v>
+      </c>
       <c r="G10" s="3">
         <v>111</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H10" s="1">
+        <v>39</v>
+      </c>
+      <c r="I10" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="5"/>
+      <c r="C11" s="6">
+        <v>831</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="E11" s="7">
+        <v>9</v>
+      </c>
+      <c r="F11" s="5">
+        <v>96</v>
+      </c>
       <c r="G11" s="3">
         <v>110</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H11" s="1">
+        <v>41</v>
+      </c>
+      <c r="I11" s="1">
+        <v>30</v>
+      </c>
+      <c r="M11" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="5"/>
+      <c r="C12" s="6">
+        <v>784</v>
+      </c>
+      <c r="D12" s="4">
+        <v>2</v>
+      </c>
+      <c r="E12" s="7">
+        <v>9</v>
+      </c>
+      <c r="F12" s="5">
+        <v>98</v>
+      </c>
       <c r="G12" s="3">
         <v>100</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H12" s="1">
+        <v>40</v>
+      </c>
+      <c r="I12" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="5"/>
+      <c r="C13" s="6">
+        <v>938</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="E13" s="7">
+        <v>9</v>
+      </c>
+      <c r="F13" s="5">
+        <v>97</v>
+      </c>
       <c r="G13" s="3">
         <v>107</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H13" s="1">
+        <v>40</v>
+      </c>
+      <c r="I13" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="5"/>
+      <c r="C14" s="6">
+        <v>822</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="E14" s="7">
+        <v>9</v>
+      </c>
+      <c r="F14" s="5">
+        <v>97</v>
+      </c>
       <c r="G14" s="3">
         <v>106</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H14" s="1">
+        <v>42</v>
+      </c>
+      <c r="I14" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="5"/>
+      <c r="C15" s="6">
+        <v>798</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E15" s="7">
+        <v>9</v>
+      </c>
+      <c r="F15" s="5">
+        <v>96</v>
+      </c>
       <c r="G15" s="3">
         <v>109</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15" s="1">
+        <v>37</v>
+      </c>
+      <c r="I15" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="5"/>
+      <c r="C16" s="6">
+        <v>760</v>
+      </c>
+      <c r="D16" s="4">
+        <v>2</v>
+      </c>
+      <c r="E16" s="7">
+        <v>9</v>
+      </c>
+      <c r="F16" s="5">
+        <v>98</v>
+      </c>
       <c r="G16" s="3">
         <v>101</v>
       </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="H16" s="1">
+        <v>36</v>
+      </c>
+      <c r="I16" s="1">
+        <v>33</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
@@ -3154,15 +3382,27 @@
       <c r="B17" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="5"/>
+      <c r="C17" s="6">
+        <v>885</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="E17" s="7">
+        <v>9</v>
+      </c>
+      <c r="F17" s="5">
+        <v>96</v>
+      </c>
       <c r="G17" s="3">
         <v>109</v>
       </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="H17" s="1">
+        <v>39</v>
+      </c>
+      <c r="I17" s="1">
+        <v>34</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -3171,15 +3411,27 @@
       <c r="B18" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="5"/>
+      <c r="C18" s="6">
+        <v>873</v>
+      </c>
+      <c r="D18" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="E18" s="7">
+        <v>9</v>
+      </c>
+      <c r="F18" s="5">
+        <v>96</v>
+      </c>
       <c r="G18" s="3">
         <v>109</v>
       </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="H18" s="1">
+        <v>38</v>
+      </c>
+      <c r="I18" s="1">
+        <v>35</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
@@ -3199,15 +3451,27 @@
       <c r="B20" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="5"/>
+      <c r="C20" s="6">
+        <v>920</v>
+      </c>
+      <c r="D20" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E20" s="7">
+        <v>10</v>
+      </c>
+      <c r="F20" s="5">
+        <v>99</v>
+      </c>
       <c r="G20" s="3">
         <v>93</v>
       </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="H20" s="1">
+        <v>44</v>
+      </c>
+      <c r="I20" s="1">
+        <v>21</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -3216,15 +3480,27 @@
       <c r="B21" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="5"/>
+      <c r="C21" s="6">
+        <v>1290</v>
+      </c>
+      <c r="D21" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="E21" s="7">
+        <v>12</v>
+      </c>
+      <c r="F21" s="5">
+        <v>94</v>
+      </c>
       <c r="G21" s="3">
         <v>115</v>
       </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="H21" s="1">
+        <v>43</v>
+      </c>
+      <c r="I21" s="1">
+        <v>31</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -3233,15 +3509,27 @@
       <c r="B22" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="5"/>
+      <c r="C22" s="6">
+        <v>1344</v>
+      </c>
+      <c r="D22" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="E22" s="7">
+        <v>12</v>
+      </c>
+      <c r="F22" s="5">
+        <v>94</v>
+      </c>
       <c r="G22" s="3">
         <v>114</v>
       </c>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
+      <c r="H22" s="1">
+        <v>42</v>
+      </c>
+      <c r="I22" s="1">
+        <v>33</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -3250,15 +3538,27 @@
       <c r="B23" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="5"/>
+      <c r="C23" s="6">
+        <v>1036</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="E23" s="7">
+        <v>11</v>
+      </c>
+      <c r="F23" s="5">
+        <v>96</v>
+      </c>
       <c r="G23" s="3">
         <v>99</v>
       </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="H23" s="1">
+        <v>41</v>
+      </c>
+      <c r="I23" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -3267,15 +3567,27 @@
       <c r="B24" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="5"/>
+      <c r="C24" s="6">
+        <v>998</v>
+      </c>
+      <c r="D24" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="E24" s="7">
+        <v>11</v>
+      </c>
+      <c r="F24" s="5">
+        <v>95</v>
+      </c>
       <c r="G24" s="3">
         <v>115</v>
       </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
+      <c r="H24" s="1">
+        <v>40</v>
+      </c>
+      <c r="I24" s="1">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3632,7 +3944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96551E4B-D0DF-400F-B6DB-43F70FA502C4}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed snowy villages not showing up on the map, fixed npcs sitting in taverns turning when the players passes nearby, further item rebalancing.
</commit_message>
<xml_diff>
--- a/Items+Troops Spreadsheets/HYW Item Balance.xlsx
+++ b/Items+Troops Spreadsheets/HYW Item Balance.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoanne\Desktop\HYW Repo\Items+Troops Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FCD007-7BD0-48D5-91FD-D1DAE592355A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D113E8A9-AA38-4AE0-9D5D-046179800F84}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="1" activeTab="2" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="4" activeTab="4" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
   </bookViews>
   <sheets>
     <sheet name="Maces" sheetId="1" r:id="rId1"/>
     <sheet name="Axes &amp; Bardiches" sheetId="2" r:id="rId2"/>
     <sheet name="Swords &amp; Daggers" sheetId="3" r:id="rId3"/>
     <sheet name="Bastard &amp; Twohanded Swords" sheetId="4" r:id="rId4"/>
-    <sheet name="Pikes &amp; Halberds &amp; Voulges" sheetId="5" r:id="rId5"/>
+    <sheet name="Pikes &amp; Halberds" sheetId="5" r:id="rId5"/>
     <sheet name="Bows" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179021"/>
@@ -2279,11 +2279,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76258844-B7FB-4720-B431-7E6F0F318E31}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2292,7 +2292,7 @@
     <col min="2" max="2" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>67</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="5">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G2" s="3">
         <v>47</v>
@@ -2350,7 +2350,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>68</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="5">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="G3" s="3">
         <v>41</v>
@@ -2379,7 +2379,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>69</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="5">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G4" s="3">
         <v>47</v>
@@ -2408,7 +2408,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="6"/>
@@ -2419,194 +2419,414 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="5"/>
+      <c r="C6" s="6">
+        <v>325</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>103</v>
+      </c>
       <c r="G6" s="3">
         <v>70</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6" s="1">
+        <v>34</v>
+      </c>
+      <c r="I6" s="1">
+        <v>19</v>
+      </c>
+      <c r="J6">
+        <f>SUM(F6:I6)</f>
+        <v>226</v>
+      </c>
+      <c r="K6">
+        <f>J6*D6^2</f>
+        <v>325.44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="5"/>
+      <c r="C7" s="6">
+        <v>488</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>100</v>
+      </c>
       <c r="G7" s="3">
         <v>95</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H7" s="1">
+        <v>28</v>
+      </c>
+      <c r="I7" s="1">
+        <v>26</v>
+      </c>
+      <c r="J7">
+        <f>SUM(F7:I7)</f>
+        <v>249</v>
+      </c>
+      <c r="K7">
+        <f>J7*D7^2</f>
+        <v>488.03999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="5"/>
+      <c r="C8" s="6">
+        <v>572</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>99</v>
+      </c>
       <c r="G8" s="3">
         <v>101</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H8" s="1">
+        <v>29</v>
+      </c>
+      <c r="I8" s="1">
+        <v>25</v>
+      </c>
+      <c r="J8">
+        <f>SUM(F8:I8)</f>
+        <v>254</v>
+      </c>
+      <c r="K8">
+        <f>J8*D8^2</f>
+        <v>571.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="5"/>
+      <c r="C9" s="6">
+        <v>488</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>100</v>
+      </c>
       <c r="G9" s="3">
         <v>95</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H9" s="1">
+        <v>29</v>
+      </c>
+      <c r="I9" s="1">
+        <v>25</v>
+      </c>
+      <c r="J9">
+        <f>SUM(F9:I9)</f>
+        <v>249</v>
+      </c>
+      <c r="K9">
+        <f>J9*D9^2</f>
+        <v>488.03999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="5"/>
+      <c r="C10" s="6">
+        <v>572</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>99</v>
+      </c>
       <c r="G10" s="3">
         <v>101</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H10" s="1">
+        <v>30</v>
+      </c>
+      <c r="I10" s="1">
+        <v>24</v>
+      </c>
+      <c r="J10">
+        <f>SUM(F10:I10)</f>
+        <v>254</v>
+      </c>
+      <c r="K10">
+        <f>J10*D10^2</f>
+        <v>571.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="5"/>
+      <c r="C11" s="6">
+        <v>400</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>102</v>
+      </c>
       <c r="G11" s="3">
         <v>81</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H11" s="1">
+        <v>28</v>
+      </c>
+      <c r="I11" s="1">
+        <v>26</v>
+      </c>
+      <c r="J11">
+        <f>SUM(F11:I11)</f>
+        <v>237</v>
+      </c>
+      <c r="K11">
+        <f>J11*D11^2</f>
+        <v>400.53000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="5"/>
+      <c r="C12" s="6">
+        <v>488</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>100</v>
+      </c>
       <c r="G12" s="3">
         <v>95</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H12" s="1">
+        <v>29</v>
+      </c>
+      <c r="I12" s="1">
+        <v>25</v>
+      </c>
+      <c r="J12">
+        <f>SUM(F12:I12)</f>
+        <v>249</v>
+      </c>
+      <c r="K12">
+        <f>J12*D12^2</f>
+        <v>488.03999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="5"/>
+      <c r="C13" s="6">
+        <v>572</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>99</v>
+      </c>
       <c r="G13" s="3">
         <v>101</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H13" s="1">
+        <v>30</v>
+      </c>
+      <c r="I13" s="1">
+        <v>24</v>
+      </c>
+      <c r="J13">
+        <f>SUM(F13:I13)</f>
+        <v>254</v>
+      </c>
+      <c r="K13">
+        <f>J13*D13^2</f>
+        <v>571.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="5"/>
+      <c r="C14" s="6">
+        <v>506</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5">
+        <v>100</v>
+      </c>
       <c r="G14" s="3">
         <v>98</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H14" s="1">
+        <v>32</v>
+      </c>
+      <c r="I14" s="1">
+        <v>28</v>
+      </c>
+      <c r="J14">
+        <f>SUM(F14:I14)</f>
+        <v>258</v>
+      </c>
+      <c r="K14">
+        <f>J14*D14^2</f>
+        <v>505.67999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="5"/>
+      <c r="C15" s="6">
+        <v>402</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
+        <v>103</v>
+      </c>
       <c r="G15" s="3">
         <v>74</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15" s="1">
+        <v>28</v>
+      </c>
+      <c r="I15" s="1">
+        <v>33</v>
+      </c>
+      <c r="J15">
+        <f>SUM(F15:I15)</f>
+        <v>238</v>
+      </c>
+      <c r="K15">
+        <f>J15*D15^2</f>
+        <v>402.22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="5"/>
+      <c r="C16" s="6">
+        <v>406</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5">
+        <v>102</v>
+      </c>
       <c r="G16" s="3">
         <v>81</v>
       </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H16" s="1">
+        <v>26</v>
+      </c>
+      <c r="I16" s="1">
+        <v>31</v>
+      </c>
+      <c r="J16">
+        <f>SUM(F16:I16)</f>
+        <v>240</v>
+      </c>
+      <c r="K16">
+        <f>J16*D16^2</f>
+        <v>405.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="6"/>
@@ -2617,294 +2837,632 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="5"/>
+      <c r="C18" s="6">
+        <v>415</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="E18" s="7">
+        <v>0</v>
+      </c>
+      <c r="F18" s="5">
+        <v>102</v>
+      </c>
       <c r="G18" s="3">
         <v>85</v>
       </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H18" s="1">
+        <v>36</v>
+      </c>
+      <c r="I18" s="1">
+        <v>21</v>
+      </c>
+      <c r="J18">
+        <f t="shared" ref="J18:J34" si="0">SUM(D18:I18)</f>
+        <v>245.3</v>
+      </c>
+      <c r="K18">
+        <f>J18*D18^2</f>
+        <v>414.55700000000007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="5"/>
+      <c r="C19" s="6">
+        <v>487</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5">
+        <v>101</v>
+      </c>
       <c r="G19" s="3">
         <v>93</v>
       </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H19" s="1">
+        <v>30</v>
+      </c>
+      <c r="I19" s="1">
+        <v>23</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>248.4</v>
+      </c>
+      <c r="K19">
+        <f>J19*D19^2</f>
+        <v>486.86399999999992</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="5"/>
+      <c r="C20" s="6">
+        <v>582</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0</v>
+      </c>
+      <c r="F20" s="5">
+        <v>99</v>
+      </c>
       <c r="G20" s="3">
         <v>103</v>
       </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H20" s="1">
+        <v>30</v>
+      </c>
+      <c r="I20" s="1">
+        <v>25</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>258.5</v>
+      </c>
+      <c r="K20">
+        <f>J20*D20^2</f>
+        <v>581.625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="5"/>
+      <c r="C21" s="6">
+        <v>508</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0</v>
+      </c>
+      <c r="F21" s="5">
+        <v>100</v>
+      </c>
       <c r="G21" s="3">
         <v>97</v>
       </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H21" s="1">
+        <v>27</v>
+      </c>
+      <c r="I21" s="1">
+        <v>34</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>259.39999999999998</v>
+      </c>
+      <c r="K21">
+        <f>J21*D21^2</f>
+        <v>508.42399999999986</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="5"/>
+      <c r="C22" s="6">
+        <v>514</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5">
+        <v>100</v>
+      </c>
       <c r="G22" s="3">
         <v>99</v>
       </c>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H22" s="1">
+        <v>28</v>
+      </c>
+      <c r="I22" s="1">
+        <v>34</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>262.39999999999998</v>
+      </c>
+      <c r="K22">
+        <f>J22*D22^2</f>
+        <v>514.30399999999986</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="5"/>
+      <c r="C23" s="6">
+        <v>582</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E23" s="7">
+        <v>0</v>
+      </c>
+      <c r="F23" s="5">
+        <v>99</v>
+      </c>
       <c r="G23" s="3">
         <v>100</v>
       </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H23" s="1">
+        <v>28</v>
+      </c>
+      <c r="I23" s="1">
+        <v>30</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>258.5</v>
+      </c>
+      <c r="K23">
+        <f>J23*D23^2</f>
+        <v>581.625</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="5"/>
+      <c r="C24" s="6">
+        <v>577</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E24" s="7">
+        <v>0</v>
+      </c>
+      <c r="F24" s="5">
+        <v>100</v>
+      </c>
       <c r="G24" s="3">
         <v>99</v>
       </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H24" s="1">
+        <v>29</v>
+      </c>
+      <c r="I24" s="1">
+        <v>27</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>256.5</v>
+      </c>
+      <c r="K24">
+        <f>J24*D24^2</f>
+        <v>577.125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="5"/>
+      <c r="C25" s="6">
+        <v>670</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="E25" s="7">
+        <v>0</v>
+      </c>
+      <c r="F25" s="5">
+        <v>97</v>
+      </c>
       <c r="G25" s="3">
         <v>107</v>
       </c>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H25" s="1">
+        <v>28</v>
+      </c>
+      <c r="I25" s="1">
+        <v>28</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>261.60000000000002</v>
+      </c>
+      <c r="K25">
+        <f>J25*D25^2</f>
+        <v>669.69600000000014</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="5"/>
+      <c r="C26" s="6">
+        <v>491</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E26" s="7">
+        <v>0</v>
+      </c>
+      <c r="F26" s="5">
+        <v>101</v>
+      </c>
       <c r="G26" s="3">
         <v>93</v>
       </c>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H26" s="1">
+        <v>29</v>
+      </c>
+      <c r="I26" s="1">
+        <v>26</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>250.4</v>
+      </c>
+      <c r="K26">
+        <f>J26*D26^2</f>
+        <v>490.78399999999993</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="4"/>
+      <c r="C27" s="6">
+        <v>491</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1.4</v>
+      </c>
       <c r="E27" s="7"/>
-      <c r="F27" s="5"/>
+      <c r="F27" s="5">
+        <v>101</v>
+      </c>
       <c r="G27" s="3">
         <v>93</v>
       </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H27" s="1">
+        <v>30</v>
+      </c>
+      <c r="I27" s="1">
+        <v>25</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>250.4</v>
+      </c>
+      <c r="K27">
+        <f>J27*D27^2</f>
+        <v>490.78399999999993</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="5"/>
+      <c r="C28" s="6">
+        <v>406</v>
+      </c>
+      <c r="D28" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="E28" s="7">
+        <v>0</v>
+      </c>
+      <c r="F28" s="5">
+        <v>102</v>
+      </c>
       <c r="G28" s="3">
         <v>83</v>
       </c>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H28" s="1">
+        <v>30</v>
+      </c>
+      <c r="I28" s="1">
+        <v>24</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>240.3</v>
+      </c>
+      <c r="K28">
+        <f>J28*D28^2</f>
+        <v>406.10700000000008</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="5"/>
+      <c r="C29" s="6">
+        <v>497</v>
+      </c>
+      <c r="D29" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E29" s="7">
+        <v>0</v>
+      </c>
+      <c r="F29" s="5">
+        <v>101</v>
+      </c>
       <c r="G29" s="3">
         <v>92</v>
       </c>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H29" s="1">
+        <v>27</v>
+      </c>
+      <c r="I29" s="1">
+        <v>32</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>253.4</v>
+      </c>
+      <c r="K29">
+        <f>J29*D29^2</f>
+        <v>496.66399999999993</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="5"/>
+      <c r="C30" s="6">
+        <v>505</v>
+      </c>
+      <c r="D30" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E30" s="7">
+        <v>0</v>
+      </c>
+      <c r="F30" s="5">
+        <v>100</v>
+      </c>
       <c r="G30" s="3">
         <v>96</v>
       </c>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H30" s="1">
+        <v>31</v>
+      </c>
+      <c r="I30" s="1">
+        <v>29</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>257.39999999999998</v>
+      </c>
+      <c r="K30">
+        <f>J30*D30^2</f>
+        <v>504.50399999999991</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="5"/>
+      <c r="C31" s="6">
+        <v>570</v>
+      </c>
+      <c r="D31" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E31" s="7">
+        <v>0</v>
+      </c>
+      <c r="F31" s="5">
+        <v>99</v>
+      </c>
       <c r="G31" s="3">
         <v>102</v>
       </c>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H31" s="1">
+        <v>31</v>
+      </c>
+      <c r="I31" s="1">
+        <v>20</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>253.5</v>
+      </c>
+      <c r="K31">
+        <f>J31*D31^2</f>
+        <v>570.375</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="5"/>
+      <c r="C32" s="6">
+        <v>406</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="E32" s="7">
+        <v>0</v>
+      </c>
+      <c r="F32" s="5">
+        <v>102</v>
+      </c>
       <c r="G32" s="3">
         <v>83</v>
       </c>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H32" s="1">
+        <v>32</v>
+      </c>
+      <c r="I32" s="1">
+        <v>22</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>240.3</v>
+      </c>
+      <c r="K32">
+        <f>J32*D32^2</f>
+        <v>406.10700000000008</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="5"/>
+      <c r="C33" s="6">
+        <v>499</v>
+      </c>
+      <c r="D33" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E33" s="7">
+        <v>0</v>
+      </c>
+      <c r="F33" s="5">
+        <v>100</v>
+      </c>
       <c r="G33" s="3">
         <v>97</v>
       </c>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H33" s="1">
+        <v>29</v>
+      </c>
+      <c r="I33" s="1">
+        <v>27</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="0"/>
+        <v>254.4</v>
+      </c>
+      <c r="K33">
+        <f>J33*D33^2</f>
+        <v>498.62399999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>97</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="5"/>
+      <c r="C34" s="6">
+        <v>577</v>
+      </c>
+      <c r="D34" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E34" s="7">
+        <v>0</v>
+      </c>
+      <c r="F34" s="5">
+        <v>99</v>
+      </c>
       <c r="G34" s="3">
         <v>102</v>
       </c>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
+      <c r="H34" s="1">
+        <v>30</v>
+      </c>
+      <c r="I34" s="1">
+        <v>24</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="0"/>
+        <v>256.5</v>
+      </c>
+      <c r="K34">
+        <f>J34*D34^2</f>
+        <v>577.125</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3596,10 +4154,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EACF69C0-A866-4A94-A569-71E0D45D66A0}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3607,7 +4165,7 @@
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3636,304 +4194,718 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>119</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="6">
+        <v>278</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>85</v>
+      </c>
+      <c r="G2" s="3">
+        <v>185</v>
+      </c>
+      <c r="H2" s="1">
+        <v>27</v>
+      </c>
+      <c r="I2" s="1">
+        <v>34</v>
+      </c>
+      <c r="J2">
+        <f>SUM(D2:I2)/1.2</f>
+        <v>277.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C3" s="6">
+        <v>283</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>85</v>
+      </c>
+      <c r="G3" s="3">
+        <v>188</v>
+      </c>
+      <c r="H3" s="1">
+        <v>29</v>
+      </c>
+      <c r="I3" s="1">
+        <v>35</v>
+      </c>
+      <c r="J3">
+        <f>SUM(D3:I3)/1.2</f>
+        <v>282.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>121</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="6">
+        <v>280</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>85</v>
+      </c>
+      <c r="G4" s="3">
+        <v>188</v>
+      </c>
+      <c r="H4" s="1">
+        <v>28</v>
+      </c>
+      <c r="I4" s="1">
+        <v>33</v>
+      </c>
+      <c r="J4">
+        <f>SUM(D4:I4)/1.2</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="6">
+        <v>275</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>85</v>
+      </c>
+      <c r="G5" s="3">
+        <v>187</v>
+      </c>
+      <c r="H5" s="1">
+        <v>22</v>
+      </c>
+      <c r="I5" s="1">
+        <v>36</v>
+      </c>
+      <c r="J5">
+        <f>SUM(D5:I5)/1.2</f>
+        <v>276.66666666666669</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>123</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="6">
+        <v>273</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>85</v>
+      </c>
+      <c r="G6" s="3">
+        <v>181</v>
+      </c>
+      <c r="H6" s="1">
+        <v>24</v>
+      </c>
+      <c r="I6" s="1">
+        <v>35</v>
+      </c>
+      <c r="J6">
+        <f>SUM(D6:I6)/1.2</f>
+        <v>272.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="6">
+        <v>275</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>85</v>
+      </c>
+      <c r="G7" s="3">
+        <v>193</v>
+      </c>
+      <c r="H7" s="1">
+        <v>19</v>
+      </c>
+      <c r="I7" s="1">
+        <v>31</v>
+      </c>
+      <c r="J7">
+        <f>SUM(D7:I7)/1.2</f>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>125</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="6">
+        <v>492</v>
+      </c>
+      <c r="D8" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="E8" s="7">
+        <v>11</v>
+      </c>
+      <c r="F8" s="5">
+        <v>78</v>
+      </c>
+      <c r="G8" s="3">
+        <v>450</v>
+      </c>
+      <c r="H8" s="1">
+        <v>18</v>
+      </c>
+      <c r="I8" s="1">
+        <v>30</v>
+      </c>
+      <c r="J8">
+        <f>SUM(D8:I8)/1.2</f>
+        <v>492.08333333333337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="6">
+        <v>341</v>
+      </c>
+      <c r="D9" s="4">
+        <v>3</v>
+      </c>
+      <c r="E9" s="7">
+        <v>9</v>
+      </c>
+      <c r="F9" s="5">
+        <v>82</v>
+      </c>
+      <c r="G9" s="3">
+        <v>255</v>
+      </c>
+      <c r="H9" s="1">
+        <v>27</v>
+      </c>
+      <c r="I9" s="1">
+        <v>33</v>
+      </c>
+      <c r="J9">
+        <f>SUM(D9:I9)/1.2</f>
+        <v>340.83333333333337</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="6">
+        <v>333</v>
+      </c>
+      <c r="D10" s="4">
+        <v>3</v>
+      </c>
+      <c r="E10" s="7">
+        <v>9</v>
+      </c>
+      <c r="F10" s="5">
+        <v>82</v>
+      </c>
+      <c r="G10" s="3">
+        <v>246</v>
+      </c>
+      <c r="H10" s="1">
+        <v>24</v>
+      </c>
+      <c r="I10" s="1">
+        <v>35</v>
+      </c>
+      <c r="J10">
+        <f>SUM(D10:I10)/1.2</f>
+        <v>332.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>128</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="6">
+        <v>406</v>
+      </c>
+      <c r="D12" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="E12" s="7">
+        <v>9</v>
+      </c>
+      <c r="F12" s="5">
+        <v>86</v>
+      </c>
+      <c r="G12" s="3">
+        <v>170</v>
+      </c>
+      <c r="H12" s="1">
+        <v>39</v>
+      </c>
+      <c r="I12" s="1">
+        <v>31</v>
+      </c>
+      <c r="J12">
+        <f>SUM(D12:I12)*1.2</f>
+        <v>406.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>129</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="6">
+        <v>428</v>
+      </c>
+      <c r="D13" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="E13" s="7">
+        <v>9</v>
+      </c>
+      <c r="F13" s="5">
+        <v>82</v>
+      </c>
+      <c r="G13" s="3">
+        <v>193</v>
+      </c>
+      <c r="H13" s="1">
+        <v>37</v>
+      </c>
+      <c r="I13" s="1">
+        <v>32</v>
+      </c>
+      <c r="J13">
+        <f>SUM(D13:I13)*1.2</f>
+        <v>427.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>130</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="6">
+        <v>423</v>
+      </c>
+      <c r="D14" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="E14" s="7">
+        <v>9</v>
+      </c>
+      <c r="F14" s="5">
+        <v>84</v>
+      </c>
+      <c r="G14" s="3">
+        <v>180</v>
+      </c>
+      <c r="H14" s="1">
+        <v>42</v>
+      </c>
+      <c r="I14" s="1">
+        <v>34</v>
+      </c>
+      <c r="J14">
+        <f>SUM(D14:I14)*1.2</f>
+        <v>423.12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>131</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="6">
+        <v>412</v>
+      </c>
+      <c r="D15" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="E15" s="7">
+        <v>9</v>
+      </c>
+      <c r="F15" s="5">
+        <v>84</v>
+      </c>
+      <c r="G15" s="3">
+        <v>180</v>
+      </c>
+      <c r="H15" s="1">
+        <v>33</v>
+      </c>
+      <c r="I15" s="1">
+        <v>34</v>
+      </c>
+      <c r="J15">
+        <f>SUM(D15:I15)*1.2</f>
+        <v>412.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>132</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="6">
+        <v>396</v>
+      </c>
+      <c r="D16" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="E16" s="7">
+        <v>9</v>
+      </c>
+      <c r="F16" s="5">
+        <v>82</v>
+      </c>
+      <c r="G16" s="3">
+        <v>190</v>
+      </c>
+      <c r="H16" s="1">
+        <v>39</v>
+      </c>
+      <c r="I16" s="1">
+        <v>36</v>
+      </c>
+      <c r="J16">
+        <f>SUM(D16:I16)*1.1</f>
+        <v>395.56000000000006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C17" s="6">
+        <v>415</v>
+      </c>
+      <c r="D17" s="4">
+        <v>3.8</v>
+      </c>
+      <c r="E17" s="7">
+        <v>9</v>
+      </c>
+      <c r="F17" s="5">
+        <v>85</v>
+      </c>
+      <c r="G17" s="3">
+        <v>173</v>
+      </c>
+      <c r="H17" s="1">
+        <v>41</v>
+      </c>
+      <c r="I17" s="1">
+        <v>34</v>
+      </c>
+      <c r="J17">
+        <f>SUM(D17:I17)*1.2</f>
+        <v>414.96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>134</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="6">
+        <v>428</v>
+      </c>
+      <c r="D18" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="E18" s="7">
+        <v>9</v>
+      </c>
+      <c r="F18" s="5">
+        <v>82</v>
+      </c>
+      <c r="G18" s="3">
+        <v>188</v>
+      </c>
+      <c r="H18" s="1">
+        <v>40</v>
+      </c>
+      <c r="I18" s="1">
+        <v>34</v>
+      </c>
+      <c r="J18">
+        <f>SUM(D18:I18)*1.2</f>
+        <v>428.03999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B19" s="2"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="6">
+        <v>417</v>
+      </c>
+      <c r="D19" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="E19" s="7">
+        <v>9</v>
+      </c>
+      <c r="F19" s="5">
+        <v>85</v>
+      </c>
+      <c r="G19" s="3">
+        <v>174</v>
+      </c>
+      <c r="H19" s="1">
+        <v>42</v>
+      </c>
+      <c r="I19" s="1">
+        <v>34</v>
+      </c>
+      <c r="J19">
+        <f>SUM(D19:I19)*1.2</f>
+        <v>417.23999999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C20" s="6">
+        <v>435</v>
+      </c>
+      <c r="D20" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="E20" s="7">
+        <v>9</v>
+      </c>
+      <c r="F20" s="5">
+        <v>82</v>
+      </c>
+      <c r="G20" s="3">
+        <v>190</v>
+      </c>
+      <c r="H20" s="1">
+        <v>43</v>
+      </c>
+      <c r="I20" s="1">
+        <v>35</v>
+      </c>
+      <c r="J20">
+        <f>SUM(D20:I20)*1.2</f>
+        <v>435.12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C21" s="6">
+        <v>436</v>
+      </c>
+      <c r="D21" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="E21" s="7">
+        <v>9</v>
+      </c>
+      <c r="F21" s="5">
+        <v>82</v>
+      </c>
+      <c r="G21" s="3">
+        <v>193</v>
+      </c>
+      <c r="H21" s="1">
+        <v>41</v>
+      </c>
+      <c r="I21" s="1">
+        <v>35</v>
+      </c>
+      <c r="J21">
+        <f>SUM(D21:I21)*1.2</f>
+        <v>436.32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>138</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="6">
+        <v>458</v>
+      </c>
+      <c r="D22" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="E22" s="7">
+        <v>9</v>
+      </c>
+      <c r="F22" s="5">
+        <v>81</v>
+      </c>
+      <c r="G22" s="3">
+        <v>209</v>
+      </c>
+      <c r="H22" s="1">
+        <v>44</v>
+      </c>
+      <c r="I22" s="1">
+        <v>35</v>
+      </c>
+      <c r="J22">
+        <f>SUM(D22:I22)*1.2</f>
+        <v>458.03999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B23" s="2"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="6">
+        <v>406</v>
+      </c>
+      <c r="D23" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="E23" s="7">
+        <v>9</v>
+      </c>
+      <c r="F23" s="5">
+        <v>84</v>
+      </c>
+      <c r="G23" s="3">
+        <v>172</v>
+      </c>
+      <c r="H23" s="1">
+        <v>43</v>
+      </c>
+      <c r="I23" s="1">
+        <v>27</v>
+      </c>
+      <c r="J23">
+        <f>SUM(D23:I23)*1.2</f>
+        <v>406.32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>140</v>
       </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="6">
+        <v>441</v>
+      </c>
+      <c r="D24" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="E24" s="7">
+        <v>9</v>
+      </c>
+      <c r="F24" s="5">
+        <v>82</v>
+      </c>
+      <c r="G24" s="3">
+        <v>192</v>
+      </c>
+      <c r="H24" s="1">
+        <v>45</v>
+      </c>
+      <c r="I24" s="1">
+        <v>36</v>
+      </c>
+      <c r="J24">
+        <f>SUM(D24:I24)*1.2</f>
+        <v>441.47999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
+      <c r="C25" s="6">
+        <v>419</v>
+      </c>
+      <c r="D25" s="4">
+        <v>4</v>
+      </c>
+      <c r="E25" s="7">
+        <v>9</v>
+      </c>
+      <c r="F25" s="5">
+        <v>82</v>
+      </c>
+      <c r="G25" s="3">
+        <v>175</v>
+      </c>
+      <c r="H25" s="1">
+        <v>46</v>
+      </c>
+      <c r="I25" s="1">
+        <v>33</v>
+      </c>
+      <c r="J25">
+        <f>SUM(D25:I25)*1.2</f>
+        <v>418.8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Added Ettenrocal's prop variants, new hood variants for the helmets, new helmet and boot models from Full Invasion OSP. Minor tweaks and fixes.
</commit_message>
<xml_diff>
--- a/Items+Troops Spreadsheets/HYW Item Balance.xlsx
+++ b/Items+Troops Spreadsheets/HYW Item Balance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoanne\Desktop\HYW Repo\Items+Troops Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D113E8A9-AA38-4AE0-9D5D-046179800F84}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FD61C6-6C22-48E4-AD69-7460EE4E3050}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="4" activeTab="4" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="3" activeTab="4" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
   </bookViews>
   <sheets>
     <sheet name="Maces" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="225">
   <si>
     <t>ID</t>
   </si>
@@ -680,6 +680,36 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>w_bill_1</t>
+  </si>
+  <si>
+    <t>w_bill_2</t>
+  </si>
+  <si>
+    <t>w_bill_3</t>
+  </si>
+  <si>
+    <t>w_bill_4</t>
+  </si>
+  <si>
+    <t>w_bec_de_corbin</t>
+  </si>
+  <si>
+    <t>w_lochaber_axe_1</t>
+  </si>
+  <si>
+    <t>w_lochaber_axe_2</t>
+  </si>
+  <si>
+    <t>w_lochaber_axe_3</t>
+  </si>
+  <si>
+    <t>w_lochaber_axe_4</t>
+  </si>
+  <si>
+    <t>w_lochaber_axe_5</t>
   </si>
 </sst>
 </file>
@@ -2448,11 +2478,11 @@
         <v>19</v>
       </c>
       <c r="J6">
-        <f>SUM(F6:I6)</f>
+        <f t="shared" ref="J6:J16" si="0">SUM(F6:I6)</f>
         <v>226</v>
       </c>
       <c r="K6">
-        <f>J6*D6^2</f>
+        <f t="shared" ref="K6:K16" si="1">J6*D6^2</f>
         <v>325.44</v>
       </c>
     </row>
@@ -2485,11 +2515,11 @@
         <v>26</v>
       </c>
       <c r="J7">
-        <f>SUM(F7:I7)</f>
+        <f t="shared" si="0"/>
         <v>249</v>
       </c>
       <c r="K7">
-        <f>J7*D7^2</f>
+        <f t="shared" si="1"/>
         <v>488.03999999999996</v>
       </c>
     </row>
@@ -2522,11 +2552,11 @@
         <v>25</v>
       </c>
       <c r="J8">
-        <f>SUM(F8:I8)</f>
+        <f t="shared" si="0"/>
         <v>254</v>
       </c>
       <c r="K8">
-        <f>J8*D8^2</f>
+        <f t="shared" si="1"/>
         <v>571.5</v>
       </c>
     </row>
@@ -2559,11 +2589,11 @@
         <v>25</v>
       </c>
       <c r="J9">
-        <f>SUM(F9:I9)</f>
+        <f t="shared" si="0"/>
         <v>249</v>
       </c>
       <c r="K9">
-        <f>J9*D9^2</f>
+        <f t="shared" si="1"/>
         <v>488.03999999999996</v>
       </c>
     </row>
@@ -2596,11 +2626,11 @@
         <v>24</v>
       </c>
       <c r="J10">
-        <f>SUM(F10:I10)</f>
+        <f t="shared" si="0"/>
         <v>254</v>
       </c>
       <c r="K10">
-        <f>J10*D10^2</f>
+        <f t="shared" si="1"/>
         <v>571.5</v>
       </c>
     </row>
@@ -2633,11 +2663,11 @@
         <v>26</v>
       </c>
       <c r="J11">
-        <f>SUM(F11:I11)</f>
+        <f t="shared" si="0"/>
         <v>237</v>
       </c>
       <c r="K11">
-        <f>J11*D11^2</f>
+        <f t="shared" si="1"/>
         <v>400.53000000000003</v>
       </c>
     </row>
@@ -2670,11 +2700,11 @@
         <v>25</v>
       </c>
       <c r="J12">
-        <f>SUM(F12:I12)</f>
+        <f t="shared" si="0"/>
         <v>249</v>
       </c>
       <c r="K12">
-        <f>J12*D12^2</f>
+        <f t="shared" si="1"/>
         <v>488.03999999999996</v>
       </c>
     </row>
@@ -2707,11 +2737,11 @@
         <v>24</v>
       </c>
       <c r="J13">
-        <f>SUM(F13:I13)</f>
+        <f t="shared" si="0"/>
         <v>254</v>
       </c>
       <c r="K13">
-        <f>J13*D13^2</f>
+        <f t="shared" si="1"/>
         <v>571.5</v>
       </c>
     </row>
@@ -2744,11 +2774,11 @@
         <v>28</v>
       </c>
       <c r="J14">
-        <f>SUM(F14:I14)</f>
+        <f t="shared" si="0"/>
         <v>258</v>
       </c>
       <c r="K14">
-        <f>J14*D14^2</f>
+        <f t="shared" si="1"/>
         <v>505.67999999999995</v>
       </c>
     </row>
@@ -2781,11 +2811,11 @@
         <v>33</v>
       </c>
       <c r="J15">
-        <f>SUM(F15:I15)</f>
+        <f t="shared" si="0"/>
         <v>238</v>
       </c>
       <c r="K15">
-        <f>J15*D15^2</f>
+        <f t="shared" si="1"/>
         <v>402.22</v>
       </c>
     </row>
@@ -2818,11 +2848,11 @@
         <v>31</v>
       </c>
       <c r="J16">
-        <f>SUM(F16:I16)</f>
+        <f t="shared" si="0"/>
         <v>240</v>
       </c>
       <c r="K16">
-        <f>J16*D16^2</f>
+        <f t="shared" si="1"/>
         <v>405.6</v>
       </c>
     </row>
@@ -2866,11 +2896,11 @@
         <v>21</v>
       </c>
       <c r="J18">
-        <f t="shared" ref="J18:J34" si="0">SUM(D18:I18)</f>
+        <f t="shared" ref="J18:J34" si="2">SUM(D18:I18)</f>
         <v>245.3</v>
       </c>
       <c r="K18">
-        <f>J18*D18^2</f>
+        <f t="shared" ref="K18:K34" si="3">J18*D18^2</f>
         <v>414.55700000000007</v>
       </c>
     </row>
@@ -2903,11 +2933,11 @@
         <v>23</v>
       </c>
       <c r="J19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>248.4</v>
       </c>
       <c r="K19">
-        <f>J19*D19^2</f>
+        <f t="shared" si="3"/>
         <v>486.86399999999992</v>
       </c>
     </row>
@@ -2940,11 +2970,11 @@
         <v>25</v>
       </c>
       <c r="J20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>258.5</v>
       </c>
       <c r="K20">
-        <f>J20*D20^2</f>
+        <f t="shared" si="3"/>
         <v>581.625</v>
       </c>
     </row>
@@ -2977,11 +3007,11 @@
         <v>34</v>
       </c>
       <c r="J21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>259.39999999999998</v>
       </c>
       <c r="K21">
-        <f>J21*D21^2</f>
+        <f t="shared" si="3"/>
         <v>508.42399999999986</v>
       </c>
     </row>
@@ -3014,11 +3044,11 @@
         <v>34</v>
       </c>
       <c r="J22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>262.39999999999998</v>
       </c>
       <c r="K22">
-        <f>J22*D22^2</f>
+        <f t="shared" si="3"/>
         <v>514.30399999999986</v>
       </c>
     </row>
@@ -3051,11 +3081,11 @@
         <v>30</v>
       </c>
       <c r="J23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>258.5</v>
       </c>
       <c r="K23">
-        <f>J23*D23^2</f>
+        <f t="shared" si="3"/>
         <v>581.625</v>
       </c>
     </row>
@@ -3088,11 +3118,11 @@
         <v>27</v>
       </c>
       <c r="J24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>256.5</v>
       </c>
       <c r="K24">
-        <f>J24*D24^2</f>
+        <f t="shared" si="3"/>
         <v>577.125</v>
       </c>
     </row>
@@ -3125,11 +3155,11 @@
         <v>28</v>
       </c>
       <c r="J25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>261.60000000000002</v>
       </c>
       <c r="K25">
-        <f>J25*D25^2</f>
+        <f t="shared" si="3"/>
         <v>669.69600000000014</v>
       </c>
     </row>
@@ -3162,11 +3192,11 @@
         <v>26</v>
       </c>
       <c r="J26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>250.4</v>
       </c>
       <c r="K26">
-        <f>J26*D26^2</f>
+        <f t="shared" si="3"/>
         <v>490.78399999999993</v>
       </c>
     </row>
@@ -3197,11 +3227,11 @@
         <v>25</v>
       </c>
       <c r="J27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>250.4</v>
       </c>
       <c r="K27">
-        <f>J27*D27^2</f>
+        <f t="shared" si="3"/>
         <v>490.78399999999993</v>
       </c>
     </row>
@@ -3234,11 +3264,11 @@
         <v>24</v>
       </c>
       <c r="J28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>240.3</v>
       </c>
       <c r="K28">
-        <f>J28*D28^2</f>
+        <f t="shared" si="3"/>
         <v>406.10700000000008</v>
       </c>
     </row>
@@ -3271,11 +3301,11 @@
         <v>32</v>
       </c>
       <c r="J29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>253.4</v>
       </c>
       <c r="K29">
-        <f>J29*D29^2</f>
+        <f t="shared" si="3"/>
         <v>496.66399999999993</v>
       </c>
     </row>
@@ -3308,11 +3338,11 @@
         <v>29</v>
       </c>
       <c r="J30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>257.39999999999998</v>
       </c>
       <c r="K30">
-        <f>J30*D30^2</f>
+        <f t="shared" si="3"/>
         <v>504.50399999999991</v>
       </c>
     </row>
@@ -3345,11 +3375,11 @@
         <v>20</v>
       </c>
       <c r="J31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>253.5</v>
       </c>
       <c r="K31">
-        <f>J31*D31^2</f>
+        <f t="shared" si="3"/>
         <v>570.375</v>
       </c>
     </row>
@@ -3382,11 +3412,11 @@
         <v>22</v>
       </c>
       <c r="J32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>240.3</v>
       </c>
       <c r="K32">
-        <f>J32*D32^2</f>
+        <f t="shared" si="3"/>
         <v>406.10700000000008</v>
       </c>
     </row>
@@ -3419,11 +3449,11 @@
         <v>27</v>
       </c>
       <c r="J33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>254.4</v>
       </c>
       <c r="K33">
-        <f>J33*D33^2</f>
+        <f t="shared" si="3"/>
         <v>498.62399999999997</v>
       </c>
     </row>
@@ -3456,11 +3486,11 @@
         <v>24</v>
       </c>
       <c r="J34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>256.5</v>
       </c>
       <c r="K34">
-        <f>J34*D34^2</f>
+        <f t="shared" si="3"/>
         <v>577.125</v>
       </c>
     </row>
@@ -4154,10 +4184,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EACF69C0-A866-4A94-A569-71E0D45D66A0}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4221,7 +4252,7 @@
         <v>34</v>
       </c>
       <c r="J2">
-        <f>SUM(D2:I2)/1.2</f>
+        <f t="shared" ref="J2:J10" si="0">SUM(D2:I2)/1.2</f>
         <v>277.5</v>
       </c>
     </row>
@@ -4252,7 +4283,7 @@
         <v>35</v>
       </c>
       <c r="J3">
-        <f>SUM(D3:I3)/1.2</f>
+        <f t="shared" si="0"/>
         <v>282.5</v>
       </c>
     </row>
@@ -4283,7 +4314,7 @@
         <v>33</v>
       </c>
       <c r="J4">
-        <f>SUM(D4:I4)/1.2</f>
+        <f t="shared" si="0"/>
         <v>280</v>
       </c>
     </row>
@@ -4314,7 +4345,7 @@
         <v>36</v>
       </c>
       <c r="J5">
-        <f>SUM(D5:I5)/1.2</f>
+        <f t="shared" si="0"/>
         <v>276.66666666666669</v>
       </c>
     </row>
@@ -4345,7 +4376,7 @@
         <v>35</v>
       </c>
       <c r="J6">
-        <f>SUM(D6:I6)/1.2</f>
+        <f t="shared" si="0"/>
         <v>272.5</v>
       </c>
     </row>
@@ -4376,7 +4407,7 @@
         <v>31</v>
       </c>
       <c r="J7">
-        <f>SUM(D7:I7)/1.2</f>
+        <f t="shared" si="0"/>
         <v>275</v>
       </c>
     </row>
@@ -4407,7 +4438,7 @@
         <v>30</v>
       </c>
       <c r="J8">
-        <f>SUM(D8:I8)/1.2</f>
+        <f t="shared" si="0"/>
         <v>492.08333333333337</v>
       </c>
     </row>
@@ -4438,7 +4469,7 @@
         <v>33</v>
       </c>
       <c r="J9">
-        <f>SUM(D9:I9)/1.2</f>
+        <f t="shared" si="0"/>
         <v>340.83333333333337</v>
       </c>
     </row>
@@ -4469,7 +4500,7 @@
         <v>35</v>
       </c>
       <c r="J10">
-        <f>SUM(D10:I10)/1.2</f>
+        <f t="shared" si="0"/>
         <v>332.5</v>
       </c>
     </row>
@@ -4655,7 +4686,7 @@
         <v>34</v>
       </c>
       <c r="J17">
-        <f>SUM(D17:I17)*1.2</f>
+        <f t="shared" ref="J17:J25" si="1">SUM(D17:I17)*1.2</f>
         <v>414.96</v>
       </c>
     </row>
@@ -4686,7 +4717,7 @@
         <v>34</v>
       </c>
       <c r="J18">
-        <f>SUM(D18:I18)*1.2</f>
+        <f t="shared" si="1"/>
         <v>428.03999999999996</v>
       </c>
     </row>
@@ -4717,7 +4748,7 @@
         <v>34</v>
       </c>
       <c r="J19">
-        <f>SUM(D19:I19)*1.2</f>
+        <f t="shared" si="1"/>
         <v>417.23999999999995</v>
       </c>
     </row>
@@ -4748,7 +4779,7 @@
         <v>35</v>
       </c>
       <c r="J20">
-        <f>SUM(D20:I20)*1.2</f>
+        <f t="shared" si="1"/>
         <v>435.12</v>
       </c>
     </row>
@@ -4779,7 +4810,7 @@
         <v>35</v>
       </c>
       <c r="J21">
-        <f>SUM(D21:I21)*1.2</f>
+        <f t="shared" si="1"/>
         <v>436.32</v>
       </c>
     </row>
@@ -4810,7 +4841,7 @@
         <v>35</v>
       </c>
       <c r="J22">
-        <f>SUM(D22:I22)*1.2</f>
+        <f t="shared" si="1"/>
         <v>458.03999999999996</v>
       </c>
     </row>
@@ -4841,7 +4872,7 @@
         <v>27</v>
       </c>
       <c r="J23">
-        <f>SUM(D23:I23)*1.2</f>
+        <f t="shared" si="1"/>
         <v>406.32</v>
       </c>
     </row>
@@ -4872,7 +4903,7 @@
         <v>36</v>
       </c>
       <c r="J24">
-        <f>SUM(D24:I24)*1.2</f>
+        <f t="shared" si="1"/>
         <v>441.47999999999996</v>
       </c>
     </row>
@@ -4903,8 +4934,318 @@
         <v>33</v>
       </c>
       <c r="J25">
-        <f>SUM(D25:I25)*1.2</f>
+        <f t="shared" si="1"/>
         <v>418.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="6">
+        <v>424</v>
+      </c>
+      <c r="D27" s="4">
+        <v>4</v>
+      </c>
+      <c r="E27" s="7">
+        <v>9</v>
+      </c>
+      <c r="F27" s="5">
+        <v>82</v>
+      </c>
+      <c r="G27" s="3">
+        <v>191</v>
+      </c>
+      <c r="H27" s="1">
+        <v>38</v>
+      </c>
+      <c r="I27" s="1">
+        <v>29</v>
+      </c>
+      <c r="J27">
+        <f>SUM(D27:I27)*1.2</f>
+        <v>423.59999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="6">
+        <v>455</v>
+      </c>
+      <c r="D28" s="4">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E28" s="7">
+        <v>9</v>
+      </c>
+      <c r="F28" s="5">
+        <v>81</v>
+      </c>
+      <c r="G28" s="3">
+        <v>207</v>
+      </c>
+      <c r="H28" s="1">
+        <v>44</v>
+      </c>
+      <c r="I28" s="1">
+        <v>34</v>
+      </c>
+      <c r="J28">
+        <f>SUM(D28:I28)*1.2</f>
+        <v>454.92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="6">
+        <v>480</v>
+      </c>
+      <c r="D29" s="4">
+        <v>4.3</v>
+      </c>
+      <c r="E29" s="7">
+        <v>9</v>
+      </c>
+      <c r="F29" s="5">
+        <v>80</v>
+      </c>
+      <c r="G29" s="3">
+        <v>233</v>
+      </c>
+      <c r="H29" s="1">
+        <v>46</v>
+      </c>
+      <c r="I29" s="1">
+        <v>36</v>
+      </c>
+      <c r="J29">
+        <f>SUM(D29:I29)*1.2</f>
+        <v>489.96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="6">
+        <v>505</v>
+      </c>
+      <c r="D30" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="E30" s="7">
+        <v>9</v>
+      </c>
+      <c r="F30" s="5">
+        <v>79</v>
+      </c>
+      <c r="G30" s="3">
+        <v>246</v>
+      </c>
+      <c r="H30" s="1">
+        <v>45</v>
+      </c>
+      <c r="I30" s="1">
+        <v>37</v>
+      </c>
+      <c r="J30">
+        <f>SUM(D30:I30)*1.2</f>
+        <v>504.59999999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="6">
+        <v>375</v>
+      </c>
+      <c r="D32" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="E32" s="7">
+        <v>9</v>
+      </c>
+      <c r="F32" s="5">
+        <v>84</v>
+      </c>
+      <c r="G32" s="3">
+        <v>154</v>
+      </c>
+      <c r="H32" s="1">
+        <v>33</v>
+      </c>
+      <c r="I32" s="1">
+        <v>29</v>
+      </c>
+      <c r="J32">
+        <f>SUM(D32:I32)*1.2</f>
+        <v>375.47999999999996</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="6">
+        <v>376</v>
+      </c>
+      <c r="D34" s="4">
+        <v>4</v>
+      </c>
+      <c r="E34" s="7">
+        <v>9</v>
+      </c>
+      <c r="F34" s="5">
+        <v>83</v>
+      </c>
+      <c r="G34" s="3">
+        <v>148</v>
+      </c>
+      <c r="H34" s="1">
+        <v>45</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <f>SUM(D34:I34)*1.3</f>
+        <v>375.7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="6">
+        <v>383</v>
+      </c>
+      <c r="D35" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="E35" s="7">
+        <v>9</v>
+      </c>
+      <c r="F35" s="5">
+        <v>83</v>
+      </c>
+      <c r="G35" s="3">
+        <v>150</v>
+      </c>
+      <c r="H35" s="1">
+        <v>48</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <f>SUM(D35:I35)*1.3</f>
+        <v>382.85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="6">
+        <v>376</v>
+      </c>
+      <c r="D36" s="4">
+        <v>4.3</v>
+      </c>
+      <c r="E36" s="7">
+        <v>9</v>
+      </c>
+      <c r="F36" s="5">
+        <v>84</v>
+      </c>
+      <c r="G36" s="3">
+        <v>146</v>
+      </c>
+      <c r="H36" s="1">
+        <v>46</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <f>SUM(D36:I36)*1.3</f>
+        <v>376.09000000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="6">
+        <v>359</v>
+      </c>
+      <c r="D37" s="4">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E37" s="7">
+        <v>9</v>
+      </c>
+      <c r="F37" s="5">
+        <v>87</v>
+      </c>
+      <c r="G37" s="3">
+        <v>129</v>
+      </c>
+      <c r="H37" s="1">
+        <v>47</v>
+      </c>
+      <c r="I37" s="1">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <f>SUM(D37:I37)*1.3</f>
+        <v>359.32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="6">
+        <v>355</v>
+      </c>
+      <c r="D38" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="E38" s="7">
+        <v>9</v>
+      </c>
+      <c r="F38" s="5">
+        <v>88</v>
+      </c>
+      <c r="G38" s="3">
+        <v>124</v>
+      </c>
+      <c r="H38" s="1">
+        <v>48</v>
+      </c>
+      <c r="I38" s="1">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <f>SUM(D38:I38)*1.3</f>
+        <v>355.16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Added New Horses - Outfitted Noble troop trees - Added Flemish subfaction and mercenaries - Added Flemish variants of some armors
</commit_message>
<xml_diff>
--- a/Items+Troops Spreadsheets/HYW Item Balance.xlsx
+++ b/Items+Troops Spreadsheets/HYW Item Balance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoanne\Desktop\HYW Repo\Items+Troops Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FD61C6-6C22-48E4-AD69-7460EE4E3050}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4984593D-B27D-4DB4-92BF-09E848DABD89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="3" activeTab="4" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="3" activeTab="6" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
   </bookViews>
   <sheets>
     <sheet name="Maces" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Bastard &amp; Twohanded Swords" sheetId="4" r:id="rId4"/>
     <sheet name="Pikes &amp; Halberds" sheetId="5" r:id="rId5"/>
     <sheet name="Bows" sheetId="6" r:id="rId6"/>
+    <sheet name="Horses" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="238">
   <si>
     <t>ID</t>
   </si>
@@ -710,6 +711,45 @@
   </si>
   <si>
     <t>w_lochaber_axe_5</t>
+  </si>
+  <si>
+    <t>Abundance</t>
+  </si>
+  <si>
+    <t>Hitpoints</t>
+  </si>
+  <si>
+    <t>Armor</t>
+  </si>
+  <si>
+    <t>Maneuver</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>Sumpter</t>
+  </si>
+  <si>
+    <t>Rouncey</t>
+  </si>
+  <si>
+    <t>Courser</t>
+  </si>
+  <si>
+    <t>Hunter</t>
+  </si>
+  <si>
+    <t>Barded</t>
+  </si>
+  <si>
+    <t>Barded Chamfrom</t>
+  </si>
+  <si>
+    <t>Charger</t>
+  </si>
+  <si>
+    <t>War Horse</t>
   </si>
 </sst>
 </file>
@@ -4186,9 +4226,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EACF69C0-A866-4A94-A569-71E0D45D66A0}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5921,4 +5961,301 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DAD396-9A3B-4E45-8468-1404C7D6E830}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="4">
+        <v>100</v>
+      </c>
+      <c r="D2" s="7">
+        <v>100</v>
+      </c>
+      <c r="E2" s="5">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>36</v>
+      </c>
+      <c r="H2" s="1">
+        <v>42</v>
+      </c>
+      <c r="I2" s="1">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <f>SUM(C2:I2)</f>
+        <v>299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="4">
+        <v>90</v>
+      </c>
+      <c r="D3" s="7">
+        <v>110</v>
+      </c>
+      <c r="E3" s="5">
+        <v>12</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>40</v>
+      </c>
+      <c r="H3" s="1">
+        <v>42</v>
+      </c>
+      <c r="I3" s="1">
+        <v>12</v>
+      </c>
+      <c r="J3">
+        <f>SUM(C3:I3)/0.9</f>
+        <v>341.11111111111109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="4">
+        <v>80</v>
+      </c>
+      <c r="D4" s="7">
+        <v>90</v>
+      </c>
+      <c r="E4" s="5">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>50</v>
+      </c>
+      <c r="H4" s="1">
+        <v>44</v>
+      </c>
+      <c r="I4" s="1">
+        <v>16</v>
+      </c>
+      <c r="J4">
+        <f>SUM(C4:I4)/0.6</f>
+        <v>493.33333333333337</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="4">
+        <v>70</v>
+      </c>
+      <c r="D5" s="7">
+        <v>120</v>
+      </c>
+      <c r="E5" s="5">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>44</v>
+      </c>
+      <c r="H5" s="1">
+        <v>42</v>
+      </c>
+      <c r="I5" s="1">
+        <v>20</v>
+      </c>
+      <c r="J5">
+        <f>SUM(C5:I5)/0.5</f>
+        <v>624</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="4">
+        <v>60</v>
+      </c>
+      <c r="D6" s="7">
+        <v>120</v>
+      </c>
+      <c r="E6" s="5">
+        <v>25</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1">
+        <v>40</v>
+      </c>
+      <c r="H6" s="1">
+        <v>40</v>
+      </c>
+      <c r="I6" s="1">
+        <v>24</v>
+      </c>
+      <c r="J6">
+        <f>SUM(C6:I6)/0.4</f>
+        <v>780</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="4">
+        <v>40</v>
+      </c>
+      <c r="D7" s="7">
+        <v>120</v>
+      </c>
+      <c r="E7" s="5">
+        <v>30</v>
+      </c>
+      <c r="F7" s="3">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1">
+        <v>38</v>
+      </c>
+      <c r="H7" s="1">
+        <v>38</v>
+      </c>
+      <c r="I7" s="1">
+        <v>26</v>
+      </c>
+      <c r="J7">
+        <f>SUM(C7:I7)/0.3</f>
+        <v>983.33333333333337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="4">
+        <v>40</v>
+      </c>
+      <c r="D8" s="7">
+        <v>120</v>
+      </c>
+      <c r="E8" s="5">
+        <v>22</v>
+      </c>
+      <c r="F8" s="3">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1">
+        <v>42</v>
+      </c>
+      <c r="H8" s="1">
+        <v>40</v>
+      </c>
+      <c r="I8" s="1">
+        <v>24</v>
+      </c>
+      <c r="J8">
+        <f>SUM(C8:I8)/0.2</f>
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="4">
+        <v>40</v>
+      </c>
+      <c r="D9" s="7">
+        <v>130</v>
+      </c>
+      <c r="E9" s="5">
+        <v>25</v>
+      </c>
+      <c r="F9" s="3">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1">
+        <v>42</v>
+      </c>
+      <c r="H9" s="1">
+        <v>40</v>
+      </c>
+      <c r="I9" s="1">
+        <v>28</v>
+      </c>
+      <c r="J9">
+        <f>SUM(C9:I9)/0.2</f>
+        <v>1540</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Updated stats of the last few missing items. - Added translations to French and English versions.
</commit_message>
<xml_diff>
--- a/Items+Troops Spreadsheets/HYW Item Balance.xlsx
+++ b/Items+Troops Spreadsheets/HYW Item Balance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoanne\Desktop\HYW Repo\Items+Troops Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4984593D-B27D-4DB4-92BF-09E848DABD89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D3ED42-1143-4195-BDE2-241E7BF1D925}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="3" activeTab="6" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="5" activeTab="6" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
   </bookViews>
   <sheets>
     <sheet name="Maces" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,10 @@
     <sheet name="Swords &amp; Daggers" sheetId="3" r:id="rId3"/>
     <sheet name="Bastard &amp; Twohanded Swords" sheetId="4" r:id="rId4"/>
     <sheet name="Pikes &amp; Halberds" sheetId="5" r:id="rId5"/>
-    <sheet name="Bows" sheetId="6" r:id="rId6"/>
-    <sheet name="Horses" sheetId="7" r:id="rId7"/>
+    <sheet name="Forks, Fauchards &amp; Glaives" sheetId="8" r:id="rId6"/>
+    <sheet name="Spears &amp; Lances" sheetId="9" r:id="rId7"/>
+    <sheet name="Bows" sheetId="6" r:id="rId8"/>
+    <sheet name="Horses" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="316">
   <si>
     <t>ID</t>
   </si>
@@ -750,6 +752,240 @@
   </si>
   <si>
     <t>War Horse</t>
+  </si>
+  <si>
+    <t>w_fauchard_1</t>
+  </si>
+  <si>
+    <t>w_fauchard_2</t>
+  </si>
+  <si>
+    <t>w_fauchard_3</t>
+  </si>
+  <si>
+    <t>w_fauchard_4</t>
+  </si>
+  <si>
+    <t>w_fauchard_5</t>
+  </si>
+  <si>
+    <t>w_fauchard_fork_1</t>
+  </si>
+  <si>
+    <t>w_fauchard_fork_2</t>
+  </si>
+  <si>
+    <t>w_fauchard_fork_3</t>
+  </si>
+  <si>
+    <t>w_fauchard_fork_4</t>
+  </si>
+  <si>
+    <t>w_glaive_1</t>
+  </si>
+  <si>
+    <t>w_glaive_2</t>
+  </si>
+  <si>
+    <t>w_glaive_3</t>
+  </si>
+  <si>
+    <t>w_glaive_4</t>
+  </si>
+  <si>
+    <t>w_glaive_5</t>
+  </si>
+  <si>
+    <t>w_glaive_6</t>
+  </si>
+  <si>
+    <t>w_glaive_7</t>
+  </si>
+  <si>
+    <t>w_glaive_8</t>
+  </si>
+  <si>
+    <t>w_glaive_burgundy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>w_poleaxe_1</t>
+  </si>
+  <si>
+    <t>w_poleaxe_2</t>
+  </si>
+  <si>
+    <t>w_poleaxe_3</t>
+  </si>
+  <si>
+    <t>w_poleaxe_english</t>
+  </si>
+  <si>
+    <t>w_polehammer_1</t>
+  </si>
+  <si>
+    <t>w_polehammer_2</t>
+  </si>
+  <si>
+    <t>w_polehammer_lucern</t>
+  </si>
+  <si>
+    <t>w_polehammer_milan</t>
+  </si>
+  <si>
+    <t>w_spear_1</t>
+  </si>
+  <si>
+    <t>w_spear_2</t>
+  </si>
+  <si>
+    <t>w_spear_3</t>
+  </si>
+  <si>
+    <t>w_spear_4</t>
+  </si>
+  <si>
+    <t>w_spear_5</t>
+  </si>
+  <si>
+    <t>w_spear_6</t>
+  </si>
+  <si>
+    <t>w_spear_7</t>
+  </si>
+  <si>
+    <t>w_spear_8</t>
+  </si>
+  <si>
+    <t>w_voulge_1</t>
+  </si>
+  <si>
+    <t>w_voulge_2</t>
+  </si>
+  <si>
+    <t>w_voulge_3</t>
+  </si>
+  <si>
+    <t>w_voulge_4</t>
+  </si>
+  <si>
+    <t>w_voulge_6</t>
+  </si>
+  <si>
+    <t>w_voulge_7</t>
+  </si>
+  <si>
+    <t>w_voulge_8</t>
+  </si>
+  <si>
+    <t>w_voulge_french</t>
+  </si>
+  <si>
+    <t>w_voulge_short</t>
+  </si>
+  <si>
+    <t>w_voulge_swiss_1</t>
+  </si>
+  <si>
+    <t>w_voulge_swiss_2</t>
+  </si>
+  <si>
+    <t>w_voulge_swiss_3</t>
+  </si>
+  <si>
+    <t>w_voulge_swiss_4</t>
+  </si>
+  <si>
+    <t>w_fork_1</t>
+  </si>
+  <si>
+    <t>w_fork_2</t>
+  </si>
+  <si>
+    <t>w_fork_3</t>
+  </si>
+  <si>
+    <t>w_guisarme_burgundy</t>
+  </si>
+  <si>
+    <t>w_partisan_1</t>
+  </si>
+  <si>
+    <t>w_partisan_2</t>
+  </si>
+  <si>
+    <t>w_partisan_3</t>
+  </si>
+  <si>
+    <t>w_partisan_4</t>
+  </si>
+  <si>
+    <t>w_ranseur_1</t>
+  </si>
+  <si>
+    <t>w_ranseur_2</t>
+  </si>
+  <si>
+    <t>w_spetum_1</t>
+  </si>
+  <si>
+    <t>w_spetum_2</t>
+  </si>
+  <si>
+    <t>w_spetum_3</t>
+  </si>
+  <si>
+    <t>w_spetum_4</t>
+  </si>
+  <si>
+    <t>w_native_spear_c</t>
+  </si>
+  <si>
+    <t>w_light_lance</t>
+  </si>
+  <si>
+    <t>w_native_spear_b</t>
+  </si>
+  <si>
+    <t>w_native_spear_f</t>
+  </si>
+  <si>
+    <t>w_lance_1</t>
+  </si>
+  <si>
+    <t>w_lance_2</t>
+  </si>
+  <si>
+    <t>w_lance_3</t>
+  </si>
+  <si>
+    <t>w_lance_4</t>
+  </si>
+  <si>
+    <t>w_lance_5</t>
+  </si>
+  <si>
+    <t>w_lance_6</t>
+  </si>
+  <si>
+    <t>w_lance_colored_english_1</t>
+  </si>
+  <si>
+    <t>w_lance_colored_english_2</t>
+  </si>
+  <si>
+    <t>w_lance_colored_english_3</t>
+  </si>
+  <si>
+    <t>w_lance_colored_french_1</t>
+  </si>
+  <si>
+    <t>w_lance_colored_french_2</t>
+  </si>
+  <si>
+    <t>w_lance_colored_french_3</t>
   </si>
 </sst>
 </file>
@@ -4224,16 +4460,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EACF69C0-A866-4A94-A569-71E0D45D66A0}">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomLeft" activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -5286,6 +5522,1029 @@
       <c r="J38">
         <f>SUM(D38:I38)*1.3</f>
         <v>355.16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="6">
+        <v>379</v>
+      </c>
+      <c r="D40" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="E40" s="7">
+        <v>9</v>
+      </c>
+      <c r="F40" s="5">
+        <v>84</v>
+      </c>
+      <c r="G40" s="3">
+        <v>179</v>
+      </c>
+      <c r="H40" s="1">
+        <v>37</v>
+      </c>
+      <c r="I40" s="1">
+        <v>32</v>
+      </c>
+      <c r="J40">
+        <f>SUM(D40:I40)*1.1</f>
+        <v>378.95000000000005</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="6">
+        <v>360</v>
+      </c>
+      <c r="D41" s="4">
+        <v>3.3</v>
+      </c>
+      <c r="E41" s="7">
+        <v>9</v>
+      </c>
+      <c r="F41" s="5">
+        <v>88</v>
+      </c>
+      <c r="G41" s="3">
+        <v>158</v>
+      </c>
+      <c r="H41" s="1">
+        <v>39</v>
+      </c>
+      <c r="I41" s="1">
+        <v>30</v>
+      </c>
+      <c r="J41">
+        <f>SUM(D41:I41)*1.1</f>
+        <v>360.03000000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="6">
+        <v>420</v>
+      </c>
+      <c r="D42" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="E42" s="7">
+        <v>12</v>
+      </c>
+      <c r="F42" s="5">
+        <v>82</v>
+      </c>
+      <c r="G42" s="3">
+        <v>188</v>
+      </c>
+      <c r="H42" s="1">
+        <v>42</v>
+      </c>
+      <c r="I42" s="1">
+        <v>23</v>
+      </c>
+      <c r="J42">
+        <f>SUM(D42:I42)*1.2</f>
+        <v>420.84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="6">
+        <v>438</v>
+      </c>
+      <c r="D43" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="E43" s="7">
+        <v>13</v>
+      </c>
+      <c r="F43" s="5">
+        <v>89</v>
+      </c>
+      <c r="G43" s="3">
+        <v>144</v>
+      </c>
+      <c r="H43" s="1">
+        <v>39</v>
+      </c>
+      <c r="I43" s="1">
+        <v>36</v>
+      </c>
+      <c r="J43">
+        <f>SUM(D43:I43)*1.35</f>
+        <v>438.07500000000005</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="6">
+        <v>380</v>
+      </c>
+      <c r="D45" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="E45" s="7">
+        <v>9</v>
+      </c>
+      <c r="F45" s="5">
+        <v>82</v>
+      </c>
+      <c r="G45" s="3">
+        <v>154</v>
+      </c>
+      <c r="H45" s="1">
+        <v>37</v>
+      </c>
+      <c r="I45" s="1">
+        <v>31</v>
+      </c>
+      <c r="J45">
+        <f>SUM(D45:I45)*1.2</f>
+        <v>379.92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" s="6">
+        <v>444</v>
+      </c>
+      <c r="D46" s="4">
+        <v>3.8</v>
+      </c>
+      <c r="E46" s="7">
+        <v>10</v>
+      </c>
+      <c r="F46" s="5">
+        <v>80</v>
+      </c>
+      <c r="G46" s="3">
+        <v>177</v>
+      </c>
+      <c r="H46" s="1">
+        <v>38</v>
+      </c>
+      <c r="I46" s="1">
+        <v>33</v>
+      </c>
+      <c r="J46">
+        <f>SUM(D46:I46)*1.3</f>
+        <v>444.34000000000003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" s="6">
+        <v>382</v>
+      </c>
+      <c r="D47" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="E47" s="7">
+        <v>9</v>
+      </c>
+      <c r="F47" s="5">
+        <v>82</v>
+      </c>
+      <c r="G47" s="3">
+        <v>150</v>
+      </c>
+      <c r="H47" s="1">
+        <v>36</v>
+      </c>
+      <c r="I47" s="1">
+        <v>38</v>
+      </c>
+      <c r="J47">
+        <f>SUM(D47:I47)*1.2</f>
+        <v>382.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="6">
+        <v>427</v>
+      </c>
+      <c r="D48" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="E48" s="7">
+        <v>10</v>
+      </c>
+      <c r="F48" s="5">
+        <v>81</v>
+      </c>
+      <c r="G48" s="3">
+        <v>163</v>
+      </c>
+      <c r="H48" s="1">
+        <v>34</v>
+      </c>
+      <c r="I48" s="1">
+        <v>37</v>
+      </c>
+      <c r="J48">
+        <f>SUM(D48:I48)*1.3</f>
+        <v>427.18000000000006</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B50" s="2"/>
+      <c r="C50" s="6">
+        <v>394</v>
+      </c>
+      <c r="D50" s="4">
+        <v>3.8</v>
+      </c>
+      <c r="E50" s="7">
+        <v>9</v>
+      </c>
+      <c r="F50" s="5">
+        <v>87</v>
+      </c>
+      <c r="G50" s="3">
+        <v>152</v>
+      </c>
+      <c r="H50" s="1">
+        <v>38</v>
+      </c>
+      <c r="I50" s="1">
+        <v>25</v>
+      </c>
+      <c r="J50">
+        <f t="shared" ref="J50:J63" si="2">SUM(D50:I50)*1.25</f>
+        <v>393.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" s="6">
+        <v>368</v>
+      </c>
+      <c r="D51" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="E51" s="7">
+        <v>9</v>
+      </c>
+      <c r="F51" s="5">
+        <v>88</v>
+      </c>
+      <c r="G51" s="3">
+        <v>140</v>
+      </c>
+      <c r="H51" s="1">
+        <v>35</v>
+      </c>
+      <c r="I51" s="1">
+        <v>19</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="2"/>
+        <v>368.125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" s="6">
+        <v>425</v>
+      </c>
+      <c r="D52" s="4">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E52" s="7">
+        <v>9</v>
+      </c>
+      <c r="F52" s="5">
+        <v>86</v>
+      </c>
+      <c r="G52" s="3">
+        <v>162</v>
+      </c>
+      <c r="H52" s="1">
+        <v>44</v>
+      </c>
+      <c r="I52" s="1">
+        <v>35</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="2"/>
+        <v>425.125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" s="6">
+        <v>421</v>
+      </c>
+      <c r="D53" s="4">
+        <v>3.8</v>
+      </c>
+      <c r="E53" s="7">
+        <v>9</v>
+      </c>
+      <c r="F53" s="5">
+        <v>85</v>
+      </c>
+      <c r="G53" s="3">
+        <v>170</v>
+      </c>
+      <c r="H53" s="1">
+        <v>40</v>
+      </c>
+      <c r="I53" s="1">
+        <v>29</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="2"/>
+        <v>421</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B54" s="2"/>
+      <c r="C54" s="6">
+        <v>399</v>
+      </c>
+      <c r="D54" s="4">
+        <v>4</v>
+      </c>
+      <c r="E54" s="7">
+        <v>9</v>
+      </c>
+      <c r="F54" s="5">
+        <v>88</v>
+      </c>
+      <c r="G54" s="3">
+        <v>149</v>
+      </c>
+      <c r="H54" s="1">
+        <v>41</v>
+      </c>
+      <c r="I54" s="1">
+        <v>28</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="2"/>
+        <v>398.75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" s="6">
+        <v>340</v>
+      </c>
+      <c r="D55" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="E55" s="7">
+        <v>9</v>
+      </c>
+      <c r="F55" s="5">
+        <v>90</v>
+      </c>
+      <c r="G55" s="3">
+        <v>100</v>
+      </c>
+      <c r="H55" s="1">
+        <v>43</v>
+      </c>
+      <c r="I55" s="1">
+        <v>26</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="2"/>
+        <v>340.25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" s="6">
+        <v>424</v>
+      </c>
+      <c r="D56" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="E56" s="7">
+        <v>9</v>
+      </c>
+      <c r="F56" s="5">
+        <v>84</v>
+      </c>
+      <c r="G56" s="3">
+        <v>177</v>
+      </c>
+      <c r="H56" s="1">
+        <v>41</v>
+      </c>
+      <c r="I56" s="1">
+        <v>24</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="2"/>
+        <v>423.625</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B57" s="2"/>
+      <c r="C57" s="6">
+        <v>471</v>
+      </c>
+      <c r="D57" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="E57" s="7">
+        <v>9</v>
+      </c>
+      <c r="F57" s="5">
+        <v>83</v>
+      </c>
+      <c r="G57" s="3">
+        <v>210</v>
+      </c>
+      <c r="H57" s="1">
+        <v>38</v>
+      </c>
+      <c r="I57" s="1">
+        <v>33</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="2"/>
+        <v>470.875</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B58" s="2"/>
+      <c r="C58" s="6">
+        <v>431</v>
+      </c>
+      <c r="D58" s="4">
+        <v>3.8</v>
+      </c>
+      <c r="E58" s="7">
+        <v>9</v>
+      </c>
+      <c r="F58" s="5">
+        <v>85</v>
+      </c>
+      <c r="G58" s="3">
+        <v>174</v>
+      </c>
+      <c r="H58" s="1">
+        <v>39</v>
+      </c>
+      <c r="I58" s="1">
+        <v>34</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="2"/>
+        <v>431</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B59" s="2"/>
+      <c r="C59" s="6">
+        <v>328</v>
+      </c>
+      <c r="D59" s="4">
+        <v>3</v>
+      </c>
+      <c r="E59" s="7">
+        <v>9</v>
+      </c>
+      <c r="F59" s="5">
+        <v>90</v>
+      </c>
+      <c r="G59" s="3">
+        <v>99</v>
+      </c>
+      <c r="H59" s="1">
+        <v>38</v>
+      </c>
+      <c r="I59" s="1">
+        <v>23</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="2"/>
+        <v>327.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B60" s="2"/>
+      <c r="C60" s="6">
+        <v>472</v>
+      </c>
+      <c r="D60" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="E60" s="7">
+        <v>9</v>
+      </c>
+      <c r="F60" s="5">
+        <v>82</v>
+      </c>
+      <c r="G60" s="3">
+        <v>213</v>
+      </c>
+      <c r="H60" s="1">
+        <v>34</v>
+      </c>
+      <c r="I60" s="1">
+        <v>35</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="2"/>
+        <v>471.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" s="6">
+        <v>507</v>
+      </c>
+      <c r="D61" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="E61" s="7">
+        <v>9</v>
+      </c>
+      <c r="F61" s="5">
+        <v>80</v>
+      </c>
+      <c r="G61" s="3">
+        <v>240</v>
+      </c>
+      <c r="H61" s="1">
+        <v>35</v>
+      </c>
+      <c r="I61" s="1">
+        <v>37</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="2"/>
+        <v>506.875</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="C62" s="6">
+        <v>463</v>
+      </c>
+      <c r="D62" s="4">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E62" s="7">
+        <v>9</v>
+      </c>
+      <c r="F62" s="5">
+        <v>83</v>
+      </c>
+      <c r="G62" s="3">
+        <v>203</v>
+      </c>
+      <c r="H62" s="1">
+        <v>36</v>
+      </c>
+      <c r="I62" s="1">
+        <v>35</v>
+      </c>
+      <c r="J62">
+        <f t="shared" si="2"/>
+        <v>462.625</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B63" s="2"/>
+      <c r="C63" s="6">
+        <v>458</v>
+      </c>
+      <c r="D63" s="4">
+        <v>4</v>
+      </c>
+      <c r="E63" s="7">
+        <v>9</v>
+      </c>
+      <c r="F63" s="5">
+        <v>84</v>
+      </c>
+      <c r="G63" s="3">
+        <v>195</v>
+      </c>
+      <c r="H63" s="1">
+        <v>38</v>
+      </c>
+      <c r="I63" s="1">
+        <v>36</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="2"/>
+        <v>457.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" s="6">
+        <v>448</v>
+      </c>
+      <c r="D65" s="4">
+        <v>4</v>
+      </c>
+      <c r="E65" s="7">
+        <v>9</v>
+      </c>
+      <c r="F65" s="5">
+        <v>83</v>
+      </c>
+      <c r="G65" s="3">
+        <v>184</v>
+      </c>
+      <c r="H65" s="1">
+        <v>42</v>
+      </c>
+      <c r="I65" s="1">
+        <v>36</v>
+      </c>
+      <c r="J65">
+        <f>SUM(D65:I65)*1.25</f>
+        <v>447.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B67" s="2"/>
+      <c r="C67" s="6">
+        <v>254</v>
+      </c>
+      <c r="D67" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="E67" s="7">
+        <v>0</v>
+      </c>
+      <c r="F67" s="5">
+        <v>88</v>
+      </c>
+      <c r="G67" s="3">
+        <v>130</v>
+      </c>
+      <c r="H67" s="1">
+        <v>30</v>
+      </c>
+      <c r="I67" s="1">
+        <v>32</v>
+      </c>
+      <c r="J67">
+        <f>SUM(D67:I67)*0.9</f>
+        <v>253.89000000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B68" s="2"/>
+      <c r="C68" s="6">
+        <v>259</v>
+      </c>
+      <c r="D68" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E68" s="7">
+        <v>0</v>
+      </c>
+      <c r="F68" s="5">
+        <v>87</v>
+      </c>
+      <c r="G68" s="3">
+        <v>137</v>
+      </c>
+      <c r="H68" s="1">
+        <v>29</v>
+      </c>
+      <c r="I68" s="1">
+        <v>33</v>
+      </c>
+      <c r="J68">
+        <f>SUM(D68:I68)*0.9</f>
+        <v>259.38</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B69" s="2"/>
+      <c r="C69" s="6">
+        <v>270</v>
+      </c>
+      <c r="D69" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="E69" s="7">
+        <v>0</v>
+      </c>
+      <c r="F69" s="5">
+        <v>85</v>
+      </c>
+      <c r="G69" s="3">
+        <v>146</v>
+      </c>
+      <c r="H69" s="1">
+        <v>31</v>
+      </c>
+      <c r="I69" s="1">
+        <v>35</v>
+      </c>
+      <c r="J69">
+        <f>SUM(D69:I69)*0.9</f>
+        <v>269.45999999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B70" s="2"/>
+      <c r="C70" s="6">
+        <v>250</v>
+      </c>
+      <c r="D70" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="E70" s="7">
+        <v>0</v>
+      </c>
+      <c r="F70" s="5">
+        <v>88</v>
+      </c>
+      <c r="G70" s="3">
+        <v>126</v>
+      </c>
+      <c r="H70" s="1">
+        <v>29</v>
+      </c>
+      <c r="I70" s="1">
+        <v>33</v>
+      </c>
+      <c r="J70">
+        <f>SUM(D70:I70)*0.9</f>
+        <v>250.29000000000002</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B72" s="2"/>
+      <c r="C72" s="6">
+        <v>250</v>
+      </c>
+      <c r="D72" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E72" s="7">
+        <v>0</v>
+      </c>
+      <c r="F72" s="5">
+        <v>88</v>
+      </c>
+      <c r="G72" s="3">
+        <v>124</v>
+      </c>
+      <c r="H72" s="1">
+        <v>26</v>
+      </c>
+      <c r="I72" s="1">
+        <v>37</v>
+      </c>
+      <c r="J72">
+        <f>SUM(D72:I72)*0.9</f>
+        <v>249.48</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B73" s="2"/>
+      <c r="C73" s="6">
+        <v>283</v>
+      </c>
+      <c r="D73" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="E73" s="7">
+        <v>0</v>
+      </c>
+      <c r="F73" s="5">
+        <v>84</v>
+      </c>
+      <c r="G73" s="3">
+        <v>167</v>
+      </c>
+      <c r="H73" s="1">
+        <v>22</v>
+      </c>
+      <c r="I73" s="1">
+        <v>39</v>
+      </c>
+      <c r="J73">
+        <f>SUM(D73:I73)*0.9</f>
+        <v>283.14000000000004</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B75" s="2"/>
+      <c r="C75" s="6">
+        <v>275</v>
+      </c>
+      <c r="D75" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E75" s="7">
+        <v>0</v>
+      </c>
+      <c r="F75" s="5">
+        <v>86</v>
+      </c>
+      <c r="G75" s="3">
+        <v>154</v>
+      </c>
+      <c r="H75" s="1">
+        <v>27</v>
+      </c>
+      <c r="I75" s="1">
+        <v>36</v>
+      </c>
+      <c r="J75">
+        <f>SUM(D75:I75)*0.9</f>
+        <v>274.68</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B76" s="2"/>
+      <c r="C76" s="6">
+        <v>278</v>
+      </c>
+      <c r="D76" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E76" s="7">
+        <v>0</v>
+      </c>
+      <c r="F76" s="5">
+        <v>85</v>
+      </c>
+      <c r="G76" s="3">
+        <v>159</v>
+      </c>
+      <c r="H76" s="1">
+        <v>28</v>
+      </c>
+      <c r="I76" s="1">
+        <v>35</v>
+      </c>
+      <c r="J76">
+        <f>SUM(D76:I76)*0.9</f>
+        <v>278.37</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B77" s="2"/>
+      <c r="C77" s="6">
+        <v>270</v>
+      </c>
+      <c r="D77" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E77" s="7">
+        <v>0</v>
+      </c>
+      <c r="F77" s="5">
+        <v>86</v>
+      </c>
+      <c r="G77" s="3">
+        <v>156</v>
+      </c>
+      <c r="H77" s="1">
+        <v>23</v>
+      </c>
+      <c r="I77" s="1">
+        <v>33</v>
+      </c>
+      <c r="J77">
+        <f>SUM(D77:I77)*0.9</f>
+        <v>270.18</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B78" s="2"/>
+      <c r="C78" s="6">
+        <v>243</v>
+      </c>
+      <c r="D78" s="4">
+        <v>2</v>
+      </c>
+      <c r="E78" s="7">
+        <v>0</v>
+      </c>
+      <c r="F78" s="5">
+        <v>88</v>
+      </c>
+      <c r="G78" s="3">
+        <v>127</v>
+      </c>
+      <c r="H78" s="1">
+        <v>22</v>
+      </c>
+      <c r="I78" s="1">
+        <v>31</v>
+      </c>
+      <c r="J78">
+        <f>SUM(D78:I78)*0.9</f>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -5294,11 +6553,1364 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE67CB9-8D30-45BB-9729-53435DBF7C02}">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="6">
+        <v>170</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="E2" s="7">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5">
+        <v>87</v>
+      </c>
+      <c r="G2" s="3">
+        <v>151</v>
+      </c>
+      <c r="H2" s="1">
+        <v>34</v>
+      </c>
+      <c r="I2">
+        <f>SUM(D2:H2)*0.6</f>
+        <v>170.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="6">
+        <v>257</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E3" s="7">
+        <v>9</v>
+      </c>
+      <c r="F3" s="5">
+        <v>88</v>
+      </c>
+      <c r="G3" s="3">
+        <v>130</v>
+      </c>
+      <c r="H3" s="1">
+        <v>32</v>
+      </c>
+      <c r="I3">
+        <f>SUM(D3:H3)*0.6</f>
+        <v>156.78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="6">
+        <v>196</v>
+      </c>
+      <c r="D4" s="4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="7">
+        <v>9</v>
+      </c>
+      <c r="F4" s="5">
+        <v>84</v>
+      </c>
+      <c r="G4" s="3">
+        <v>196</v>
+      </c>
+      <c r="H4" s="1">
+        <v>35</v>
+      </c>
+      <c r="I4">
+        <f>SUM(D4:H4)*0.6</f>
+        <v>196.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="6">
+        <v>190</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="E5" s="7">
+        <v>9</v>
+      </c>
+      <c r="F5" s="5">
+        <v>85</v>
+      </c>
+      <c r="G5" s="3">
+        <v>183</v>
+      </c>
+      <c r="H5" s="1">
+        <v>37</v>
+      </c>
+      <c r="I5">
+        <f>SUM(D5:H5)*0.6</f>
+        <v>190.01999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="6">
+        <v>179</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="E6" s="7">
+        <v>9</v>
+      </c>
+      <c r="F6" s="5">
+        <v>86</v>
+      </c>
+      <c r="G6" s="3">
+        <v>169</v>
+      </c>
+      <c r="H6" s="1">
+        <v>31</v>
+      </c>
+      <c r="I6">
+        <f>SUM(D6:H6)*0.6</f>
+        <v>178.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="6">
+        <v>180</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="E8" s="7">
+        <v>9</v>
+      </c>
+      <c r="F8" s="5">
+        <v>86</v>
+      </c>
+      <c r="G8" s="3">
+        <v>167</v>
+      </c>
+      <c r="H8" s="1">
+        <v>36</v>
+      </c>
+      <c r="I8">
+        <f>SUM(D8:H8)*0.6</f>
+        <v>180.29999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="6">
+        <v>183</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="E9" s="7">
+        <v>9</v>
+      </c>
+      <c r="F9" s="5">
+        <v>85</v>
+      </c>
+      <c r="G9" s="3">
+        <v>173</v>
+      </c>
+      <c r="H9" s="1">
+        <v>35</v>
+      </c>
+      <c r="I9">
+        <f>SUM(D9:H9)*0.6</f>
+        <v>182.76000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="6">
+        <v>184</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="E10" s="7">
+        <v>9</v>
+      </c>
+      <c r="F10" s="5">
+        <v>85</v>
+      </c>
+      <c r="G10" s="3">
+        <v>177</v>
+      </c>
+      <c r="H10" s="1">
+        <v>34</v>
+      </c>
+      <c r="I10">
+        <f>SUM(D10:H10)*0.6</f>
+        <v>184.43999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="6">
+        <v>166</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="E11" s="7">
+        <v>9</v>
+      </c>
+      <c r="F11" s="5">
+        <v>87</v>
+      </c>
+      <c r="G11" s="3">
+        <v>147</v>
+      </c>
+      <c r="H11" s="1">
+        <v>32</v>
+      </c>
+      <c r="I11">
+        <f>SUM(D11:H11)*0.6</f>
+        <v>166.26000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="6">
+        <v>241</v>
+      </c>
+      <c r="D13" s="4">
+        <v>3</v>
+      </c>
+      <c r="E13" s="7">
+        <v>9</v>
+      </c>
+      <c r="F13" s="5">
+        <v>83</v>
+      </c>
+      <c r="G13" s="3">
+        <v>174</v>
+      </c>
+      <c r="H13" s="1">
+        <v>32</v>
+      </c>
+      <c r="I13">
+        <f t="shared" ref="I13:I20" si="0">SUM(D13:H13)*0.8</f>
+        <v>240.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="6">
+        <v>242</v>
+      </c>
+      <c r="D14" s="4">
+        <v>3</v>
+      </c>
+      <c r="E14" s="7">
+        <v>9</v>
+      </c>
+      <c r="F14" s="5">
+        <v>83</v>
+      </c>
+      <c r="G14" s="3">
+        <v>175</v>
+      </c>
+      <c r="H14" s="1">
+        <v>33</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>242.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="6">
+        <v>304</v>
+      </c>
+      <c r="D15" s="4">
+        <v>4</v>
+      </c>
+      <c r="E15" s="7">
+        <v>9</v>
+      </c>
+      <c r="F15" s="5">
+        <v>78</v>
+      </c>
+      <c r="G15" s="3">
+        <v>255</v>
+      </c>
+      <c r="H15" s="1">
+        <v>34</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>304</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="6">
+        <v>246</v>
+      </c>
+      <c r="D16" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="E16" s="7">
+        <v>9</v>
+      </c>
+      <c r="F16" s="5">
+        <v>82</v>
+      </c>
+      <c r="G16" s="3">
+        <v>179</v>
+      </c>
+      <c r="H16" s="1">
+        <v>34</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>245.76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="6">
+        <v>251</v>
+      </c>
+      <c r="D17" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="E17" s="7">
+        <v>9</v>
+      </c>
+      <c r="F17" s="5">
+        <v>82</v>
+      </c>
+      <c r="G17" s="3">
+        <v>185</v>
+      </c>
+      <c r="H17" s="1">
+        <v>35</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>251.36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="6">
+        <v>233</v>
+      </c>
+      <c r="D18" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="E18" s="7">
+        <v>9</v>
+      </c>
+      <c r="F18" s="5">
+        <v>84</v>
+      </c>
+      <c r="G18" s="3">
+        <v>160</v>
+      </c>
+      <c r="H18" s="1">
+        <v>36</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>233.44000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="6">
+        <v>233</v>
+      </c>
+      <c r="D19" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="E19" s="7">
+        <v>9</v>
+      </c>
+      <c r="F19" s="5">
+        <v>84</v>
+      </c>
+      <c r="G19" s="3">
+        <v>164</v>
+      </c>
+      <c r="H19" s="1">
+        <v>31</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>232.64000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="6">
+        <v>268</v>
+      </c>
+      <c r="D20" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="E20" s="7">
+        <v>9</v>
+      </c>
+      <c r="F20" s="5">
+        <v>80</v>
+      </c>
+      <c r="G20" s="3">
+        <v>208</v>
+      </c>
+      <c r="H20" s="1">
+        <v>35</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>268.48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="6">
+        <v>295</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="E21" s="7">
+        <v>9</v>
+      </c>
+      <c r="F21" s="5">
+        <v>84</v>
+      </c>
+      <c r="G21" s="3">
+        <v>160</v>
+      </c>
+      <c r="H21" s="1">
+        <v>39</v>
+      </c>
+      <c r="I21">
+        <f>SUM(D21:H21)</f>
+        <v>294.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="6">
+        <v>231</v>
+      </c>
+      <c r="D23" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="E23" s="7">
+        <v>9</v>
+      </c>
+      <c r="F23" s="5">
+        <v>85</v>
+      </c>
+      <c r="G23" s="3">
+        <v>155</v>
+      </c>
+      <c r="H23" s="1">
+        <v>36</v>
+      </c>
+      <c r="I23">
+        <f>SUM(D23:H23)*0.8</f>
+        <v>230.48000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{270FCD42-7C0A-42FB-9872-27F0BB063FAE}">
+  <dimension ref="A1:I32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="6">
+        <v>134</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>99</v>
+      </c>
+      <c r="G2" s="3">
+        <v>107</v>
+      </c>
+      <c r="H2" s="1">
+        <v>37</v>
+      </c>
+      <c r="I2">
+        <f>SUM(D2:H2)*0.55</f>
+        <v>134.255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="6">
+        <v>144</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>97</v>
+      </c>
+      <c r="G3" s="3">
+        <v>128</v>
+      </c>
+      <c r="H3" s="1">
+        <v>36</v>
+      </c>
+      <c r="I3">
+        <f>SUM(D3:H3)*0.55</f>
+        <v>144.26500000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="6">
+        <v>146</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>97</v>
+      </c>
+      <c r="G4" s="3">
+        <v>132</v>
+      </c>
+      <c r="H4" s="1">
+        <v>36</v>
+      </c>
+      <c r="I4">
+        <f>SUM(D4:H4)*0.55</f>
+        <v>146.46500000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="6">
+        <v>165</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>96</v>
+      </c>
+      <c r="G5" s="3">
+        <v>142</v>
+      </c>
+      <c r="H5" s="1">
+        <v>35</v>
+      </c>
+      <c r="I5">
+        <f>SUM(D5:H5)*0.6</f>
+        <v>164.64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="6">
+        <v>166</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>96</v>
+      </c>
+      <c r="G6" s="3">
+        <v>144</v>
+      </c>
+      <c r="H6" s="1">
+        <v>35</v>
+      </c>
+      <c r="I6">
+        <f>SUM(D6:H6)*0.6</f>
+        <v>165.83999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="6">
+        <v>168</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>95</v>
+      </c>
+      <c r="G7" s="3">
+        <v>149</v>
+      </c>
+      <c r="H7" s="1">
+        <v>34</v>
+      </c>
+      <c r="I7">
+        <f>SUM(D7:H7)*0.6</f>
+        <v>167.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="6">
+        <v>229</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>90</v>
+      </c>
+      <c r="G8" s="3">
+        <v>204</v>
+      </c>
+      <c r="H8" s="1">
+        <v>31</v>
+      </c>
+      <c r="I8">
+        <f>SUM(D8:H8)*0.7</f>
+        <v>228.89999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="6">
+        <v>117</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>100</v>
+      </c>
+      <c r="G9" s="3">
+        <v>95</v>
+      </c>
+      <c r="H9" s="1">
+        <v>38</v>
+      </c>
+      <c r="I9">
+        <f>SUM(D9:H9)*0.5</f>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="6">
+        <v>87</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>87</v>
+      </c>
+      <c r="G11" s="3">
+        <v>135</v>
+      </c>
+      <c r="H11" s="1">
+        <v>26</v>
+      </c>
+      <c r="I11">
+        <f>SUM(D11:H11)*0.35</f>
+        <v>87.324999999999989</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="6">
+        <v>84</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>88</v>
+      </c>
+      <c r="G12" s="3">
+        <v>126</v>
+      </c>
+      <c r="H12" s="1">
+        <v>25</v>
+      </c>
+      <c r="I12">
+        <f>SUM(D12:H12)*0.35</f>
+        <v>84.14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="6">
+        <v>142</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>84</v>
+      </c>
+      <c r="G13" s="3">
+        <v>168</v>
+      </c>
+      <c r="H13" s="1">
+        <v>31</v>
+      </c>
+      <c r="I13">
+        <f>SUM(D13:H13)*0.5</f>
+        <v>142.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="6">
+        <v>285</v>
+      </c>
+      <c r="D15" s="4">
+        <v>3</v>
+      </c>
+      <c r="E15" s="7">
+        <v>9</v>
+      </c>
+      <c r="F15" s="5">
+        <v>84</v>
+      </c>
+      <c r="G15" s="3">
+        <v>355</v>
+      </c>
+      <c r="H15" s="1">
+        <v>25</v>
+      </c>
+      <c r="I15">
+        <f>SUM(D15:H15)*0.6</f>
+        <v>285.59999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="6">
+        <v>214</v>
+      </c>
+      <c r="D16" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="E16" s="7">
+        <v>9</v>
+      </c>
+      <c r="F16" s="5">
+        <v>92</v>
+      </c>
+      <c r="G16" s="3">
+        <v>175</v>
+      </c>
+      <c r="H16" s="1">
+        <v>27</v>
+      </c>
+      <c r="I16">
+        <f>SUM(D16:H16)*0.7</f>
+        <v>213.85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="6">
+        <v>224</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="E17" s="7">
+        <v>9</v>
+      </c>
+      <c r="F17" s="5">
+        <v>90</v>
+      </c>
+      <c r="G17" s="3">
+        <v>190</v>
+      </c>
+      <c r="H17" s="1">
+        <v>29</v>
+      </c>
+      <c r="I17">
+        <f>SUM(D17:H17)*0.7</f>
+        <v>224.27999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="6">
+        <v>320</v>
+      </c>
+      <c r="D19" s="4">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E19" s="7">
+        <v>12</v>
+      </c>
+      <c r="F19" s="5">
+        <v>82</v>
+      </c>
+      <c r="G19" s="3">
+        <v>267</v>
+      </c>
+      <c r="H19" s="1">
+        <v>35</v>
+      </c>
+      <c r="I19">
+        <f>SUM(D19:H19)*0.8</f>
+        <v>320.32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="6">
+        <v>286</v>
+      </c>
+      <c r="D20" s="4">
+        <v>4</v>
+      </c>
+      <c r="E20" s="7">
+        <v>12</v>
+      </c>
+      <c r="F20" s="5">
+        <v>85</v>
+      </c>
+      <c r="G20" s="3">
+        <v>226</v>
+      </c>
+      <c r="H20" s="1">
+        <v>31</v>
+      </c>
+      <c r="I20">
+        <f>SUM(D20:H20)*0.8</f>
+        <v>286.40000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="6">
+        <v>307</v>
+      </c>
+      <c r="D21" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="E21" s="7">
+        <v>12</v>
+      </c>
+      <c r="F21" s="5">
+        <v>83</v>
+      </c>
+      <c r="G21" s="3">
+        <v>253</v>
+      </c>
+      <c r="H21" s="1">
+        <v>32</v>
+      </c>
+      <c r="I21">
+        <f>SUM(D21:H21)*0.8</f>
+        <v>307.36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="6">
+        <v>307</v>
+      </c>
+      <c r="D22" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="E22" s="7">
+        <v>12</v>
+      </c>
+      <c r="F22" s="5">
+        <v>83</v>
+      </c>
+      <c r="G22" s="3">
+        <v>253</v>
+      </c>
+      <c r="H22" s="1">
+        <v>32</v>
+      </c>
+      <c r="I22">
+        <f>SUM(D22:H22)*0.8</f>
+        <v>307.36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="6">
+        <v>308</v>
+      </c>
+      <c r="D23" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="E23" s="7">
+        <v>12</v>
+      </c>
+      <c r="F23" s="5">
+        <v>83</v>
+      </c>
+      <c r="G23" s="3">
+        <v>252</v>
+      </c>
+      <c r="H23" s="1">
+        <v>34</v>
+      </c>
+      <c r="I23">
+        <f>SUM(D23:H23)*0.8</f>
+        <v>308.16000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="6">
+        <v>296</v>
+      </c>
+      <c r="D24" s="4">
+        <v>4.3</v>
+      </c>
+      <c r="E24" s="7">
+        <v>12</v>
+      </c>
+      <c r="F24" s="5">
+        <v>83</v>
+      </c>
+      <c r="G24" s="3">
+        <v>241</v>
+      </c>
+      <c r="H24" s="1">
+        <v>30</v>
+      </c>
+      <c r="I24">
+        <f>SUM(D24:H24)*0.8</f>
+        <v>296.24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="6">
+        <v>308</v>
+      </c>
+      <c r="D26" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="E26" s="7">
+        <v>12</v>
+      </c>
+      <c r="F26" s="5">
+        <v>83</v>
+      </c>
+      <c r="G26" s="3">
+        <v>252</v>
+      </c>
+      <c r="H26" s="1">
+        <v>34</v>
+      </c>
+      <c r="I26">
+        <f>SUM(D26:H26)*0.8</f>
+        <v>308.16000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="6">
+        <v>308</v>
+      </c>
+      <c r="D27" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="E27" s="7">
+        <v>12</v>
+      </c>
+      <c r="F27" s="5">
+        <v>83</v>
+      </c>
+      <c r="G27" s="3">
+        <v>252</v>
+      </c>
+      <c r="H27" s="1">
+        <v>34</v>
+      </c>
+      <c r="I27">
+        <f>SUM(D27:H27)*0.8</f>
+        <v>308.16000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="6">
+        <v>320</v>
+      </c>
+      <c r="D28" s="4">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E28" s="7">
+        <v>12</v>
+      </c>
+      <c r="F28" s="5">
+        <v>82</v>
+      </c>
+      <c r="G28" s="3">
+        <v>267</v>
+      </c>
+      <c r="H28" s="1">
+        <v>35</v>
+      </c>
+      <c r="I28">
+        <f>SUM(D28:H28)*0.8</f>
+        <v>320.32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="6">
+        <v>308</v>
+      </c>
+      <c r="D30" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="E30" s="7">
+        <v>12</v>
+      </c>
+      <c r="F30" s="5">
+        <v>83</v>
+      </c>
+      <c r="G30" s="3">
+        <v>252</v>
+      </c>
+      <c r="H30" s="1">
+        <v>34</v>
+      </c>
+      <c r="I30">
+        <f>SUM(D30:H30)*0.8</f>
+        <v>308.16000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="6">
+        <v>308</v>
+      </c>
+      <c r="D31" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="E31" s="7">
+        <v>12</v>
+      </c>
+      <c r="F31" s="5">
+        <v>83</v>
+      </c>
+      <c r="G31" s="3">
+        <v>252</v>
+      </c>
+      <c r="H31" s="1">
+        <v>34</v>
+      </c>
+      <c r="I31">
+        <f>SUM(D31:H31)*0.8</f>
+        <v>308.16000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="6">
+        <v>308</v>
+      </c>
+      <c r="D32" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="E32" s="7">
+        <v>12</v>
+      </c>
+      <c r="F32" s="5">
+        <v>83</v>
+      </c>
+      <c r="G32" s="3">
+        <v>252</v>
+      </c>
+      <c r="H32" s="1">
+        <v>34</v>
+      </c>
+      <c r="I32">
+        <f>SUM(D32:H32)*0.8</f>
+        <v>308.16000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96551E4B-D0DF-400F-B6DB-43F70FA502C4}">
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5679,7 +8291,7 @@
         <v>80</v>
       </c>
       <c r="G17" s="3">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="H17" s="1">
         <v>98</v>
@@ -5706,7 +8318,7 @@
         <v>79</v>
       </c>
       <c r="G18" s="3">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="H18" s="1">
         <v>98</v>
@@ -5733,7 +8345,7 @@
         <v>78</v>
       </c>
       <c r="G19" s="3">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="H19" s="1">
         <v>99</v>
@@ -5760,7 +8372,7 @@
         <v>77</v>
       </c>
       <c r="G20" s="3">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="H20" s="1">
         <v>99</v>
@@ -5841,7 +8453,7 @@
         <v>72</v>
       </c>
       <c r="G24" s="3">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="H24" s="1">
         <v>99</v>
@@ -5868,7 +8480,7 @@
         <v>68</v>
       </c>
       <c r="G25" s="3">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="H25" s="1">
         <v>99</v>
@@ -5895,7 +8507,7 @@
         <v>62</v>
       </c>
       <c r="G26" s="3">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="H26" s="1">
         <v>98</v>
@@ -5963,11 +8575,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DAD396-9A3B-4E45-8468-1404C7D6E830}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>

</xml_diff>